<commit_message>
Added Other Info import fields
</commit_message>
<xml_diff>
--- a/django_api/django_api/apps/unicef/templates/excel/hr_export.xlsx
+++ b/django_api/django_api/apps/unicef/templates/excel/hr_export.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dariuszfryta/work/prp/django_api/django_api/apps/unicef/templates/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C332051-30AC-6C40-959E-EF99727F95E2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B32E71-B055-BB47-B9B3-6095F19FD27A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -355,7 +355,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -390,6 +390,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -675,9 +681,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM956"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AM1" sqref="AM1:AM1048576"/>
+      <selection pane="bottomLeft" activeCell="J5" activeCellId="2" sqref="M5 L5 J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -711,9 +717,9 @@
     <col min="33" max="34" width="16.83203125" customWidth="1"/>
     <col min="35" max="35" width="21.5" customWidth="1"/>
     <col min="36" max="36" width="21" customWidth="1"/>
-    <col min="37" max="37" width="25.1640625" customWidth="1"/>
-    <col min="38" max="38" width="16.83203125" customWidth="1"/>
-    <col min="39" max="39" width="18.6640625" customWidth="1"/>
+    <col min="37" max="37" width="25.1640625" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="16.83203125" hidden="1" customWidth="1"/>
+    <col min="39" max="39" width="18.6640625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1010,10 +1016,10 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
+      <c r="J5" s="16"/>
       <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="5"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="15"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
       <c r="P5" s="4"/>
@@ -40035,5 +40041,6 @@
   </sheetData>
   <autoFilter ref="A1:AM956" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: PR Export adjustments [ch12257] [ch12299] [ch12304] [ch12312]
+ sheet_no adjustment after appending or removing sheets

+ Cell Fill style for all disaggregated data columns and QPR Other Info columns

+ hr_export template file updates

+ Updated import_export module to set QPR info columns from NoneType

+ Added integer conversion on disaggregated data value

+ Added logic to update narrative assessment at Indicator Report per PD Output level
</commit_message>
<xml_diff>
--- a/django_api/django_api/apps/unicef/templates/excel/hr_export.xlsx
+++ b/django_api/django_api/apps/unicef/templates/excel/hr_export.xlsx
@@ -16,16 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
-    <t>Please note that this sheet is specifically designed to report on a particular report.</t>
-  </si>
-  <si>
     <t>Partner Name</t>
-  </si>
-  <si>
-    <t>If you generated this sheet for QPR 1, then please use it only for that report. Do not re-use it on any other reports.</t>
-  </si>
-  <si>
-    <t>Things to do:</t>
   </si>
   <si>
     <t>Country</t>
@@ -35,6 +26,9 @@
   </si>
   <si>
     <t>PD Title</t>
+  </si>
+  <si>
+    <t>Please note that this sheet is specifically designed to report on a particular report.</t>
   </si>
   <si>
     <t>PD Output Title</t>
@@ -55,31 +49,13 @@
     <t>Partner contribution to date (for entire report)</t>
   </si>
   <si>
-    <t>* Fill in only the the fields that are marked in orange</t>
-  </si>
-  <si>
-    <t>For percentage and ratio indicators, simply enter the numbers with a slash, e.g: 15/100</t>
-  </si>
-  <si>
-    <t>Insert Partner contribution to date, Challenges/bottlenecks in the reporting period and Proposed way forward only once on 1 sheet. You do not have to repeat it.</t>
-  </si>
-  <si>
-    <t>Do not:</t>
-  </si>
-  <si>
     <t>Funds received to date</t>
-  </si>
-  <si>
-    <t>Add or delete any sheets, rows or columns</t>
   </si>
   <si>
     <t>Challenges/bottlenecks in the reporting period (for entire report)</t>
   </si>
   <si>
     <t>Proposed way forward (for entire report)</t>
-  </si>
-  <si>
-    <t>Overwrite any cells that are generated by the system</t>
   </si>
   <si>
     <t>Submitted by</t>
@@ -133,6 +109,9 @@
     <t>Location Admin Level 3</t>
   </si>
   <si>
+    <t>If you generated this sheet for QPR 1, then please use it only for that report. Do not re-use it on any other reports.</t>
+  </si>
+  <si>
     <t>Admin Level 3 PCode</t>
   </si>
   <si>
@@ -154,6 +133,9 @@
     <t>Denominator Label (for percentage and ratio indicators)</t>
   </si>
   <si>
+    <t>Things to do:</t>
+  </si>
+  <si>
     <t>Achievement in reporting period (total across all locations)</t>
   </si>
   <si>
@@ -163,10 +145,28 @@
     <t>Progress Report ID</t>
   </si>
   <si>
+    <t>* Fill in only the the fields that are marked in orange</t>
+  </si>
+  <si>
+    <t>For percentage and ratio indicators, simply enter the numbers with a slash, e.g: 15/100</t>
+  </si>
+  <si>
+    <t>Insert Partner contribution to date, Challenges/bottlenecks in the reporting period and Proposed way forward only once on 1 sheet. You do not have to repeat it.</t>
+  </si>
+  <si>
     <t>Indicator ID</t>
   </si>
   <si>
     <t>Location ID</t>
+  </si>
+  <si>
+    <t>Do not:</t>
+  </si>
+  <si>
+    <t>Add or delete any sheets, rows or columns</t>
+  </si>
+  <si>
+    <t>Overwrite any cells that are generated by the system</t>
   </si>
   <si>
     <t>#partner+name</t>
@@ -306,16 +306,16 @@
       <name val="Arial"/>
     </font>
     <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="12.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font/>
-    <font>
-      <b/>
-      <sz val="11.0"/>
-      <name val="Calibri"/>
-    </font>
     <font>
       <b/>
       <sz val="14.0"/>
@@ -369,30 +369,30 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
@@ -421,20 +421,16 @@
     <xf borderId="0" fillId="0" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="2" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="9" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -465,70 +461,70 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+      <c r="A1" s="2" t="s">
+        <v>4</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="4"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
+      <c r="A2" s="2" t="s">
+        <v>31</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="4"/>
     </row>
     <row r="3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
+      <c r="A4" s="5" t="s">
+        <v>39</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="4"/>
     </row>
     <row r="5">
-      <c r="A5" s="5"/>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
+      <c r="A5" s="7"/>
+      <c r="B5" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
+      <c r="A6" s="2" t="s">
+        <v>44</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="4"/>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
+      <c r="A7" s="2" t="s">
+        <v>45</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="4"/>
     </row>
     <row r="8">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
     </row>
     <row r="9">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="s">
-        <v>16</v>
+      <c r="A10" s="5" t="s">
+        <v>48</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="4"/>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="s">
-        <v>18</v>
+      <c r="A11" s="2" t="s">
+        <v>49</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="4"/>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="s">
-        <v>21</v>
+      <c r="A12" s="2" t="s">
+        <v>50</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -583,131 +579,131 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>4</v>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="L1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="R1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="T1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="U1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="W1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="X1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Y1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="Z1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="AA1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="AB1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="AC1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="AD1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="X1" s="3" t="s">
+      <c r="AE1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AF1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AG1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AH1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AI1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AE1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AL1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AM1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AN1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="AI1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AJ1" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AK1" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AO1" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="AM1" s="7" t="s">
+      <c r="AP1" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="AN1" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="AO1" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="AP1" s="8" t="s">
-        <v>50</v>
       </c>
       <c r="AQ1" s="9"/>
       <c r="AR1" s="9"/>
@@ -1025,7 +1021,7 @@
       <c r="P5" s="21"/>
       <c r="Q5" s="21"/>
       <c r="R5" s="18"/>
-      <c r="S5" s="22"/>
+      <c r="S5" s="18"/>
       <c r="T5" s="18"/>
       <c r="U5" s="18"/>
       <c r="V5" s="18"/>
@@ -1042,13 +1038,13 @@
       <c r="AG5" s="21"/>
       <c r="AH5" s="18"/>
       <c r="AI5" s="18"/>
-      <c r="AJ5" s="23"/>
-      <c r="AK5" s="23"/>
-      <c r="AL5" s="24"/>
+      <c r="AJ5" s="22"/>
+      <c r="AK5" s="22"/>
+      <c r="AL5" s="21"/>
       <c r="AM5" s="18"/>
-      <c r="AN5" s="25"/>
-      <c r="AO5" s="25"/>
-      <c r="AP5" s="25"/>
+      <c r="AN5" s="23"/>
+      <c r="AO5" s="23"/>
+      <c r="AP5" s="23"/>
       <c r="AQ5" s="10"/>
       <c r="AR5" s="10"/>
       <c r="AS5" s="10"/>
@@ -1080,10 +1076,10 @@
       <c r="G6" s="18"/>
       <c r="H6" s="18"/>
       <c r="I6" s="18"/>
-      <c r="J6" s="22"/>
+      <c r="J6" s="18"/>
       <c r="K6" s="18"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="24"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="21"/>
       <c r="N6" s="21"/>
       <c r="O6" s="21"/>
       <c r="P6" s="21"/>
@@ -1110,9 +1106,9 @@
       <c r="AK6" s="18"/>
       <c r="AL6" s="21"/>
       <c r="AM6" s="18"/>
-      <c r="AN6" s="25"/>
-      <c r="AO6" s="25"/>
-      <c r="AP6" s="25"/>
+      <c r="AN6" s="23"/>
+      <c r="AO6" s="23"/>
+      <c r="AP6" s="23"/>
       <c r="AQ6" s="10"/>
       <c r="AR6" s="10"/>
       <c r="AS6" s="10"/>
@@ -1174,9 +1170,9 @@
       <c r="AK7" s="18"/>
       <c r="AL7" s="21"/>
       <c r="AM7" s="18"/>
-      <c r="AN7" s="25"/>
-      <c r="AO7" s="25"/>
-      <c r="AP7" s="25"/>
+      <c r="AN7" s="23"/>
+      <c r="AO7" s="23"/>
+      <c r="AP7" s="23"/>
       <c r="AQ7" s="10"/>
       <c r="AR7" s="10"/>
       <c r="AS7" s="10"/>
@@ -1238,9 +1234,9 @@
       <c r="AK8" s="18"/>
       <c r="AL8" s="21"/>
       <c r="AM8" s="18"/>
-      <c r="AN8" s="25"/>
-      <c r="AO8" s="25"/>
-      <c r="AP8" s="25"/>
+      <c r="AN8" s="23"/>
+      <c r="AO8" s="23"/>
+      <c r="AP8" s="23"/>
       <c r="AQ8" s="10"/>
       <c r="AR8" s="10"/>
       <c r="AS8" s="10"/>
@@ -1302,9 +1298,9 @@
       <c r="AK9" s="18"/>
       <c r="AL9" s="21"/>
       <c r="AM9" s="18"/>
-      <c r="AN9" s="25"/>
-      <c r="AO9" s="25"/>
-      <c r="AP9" s="25"/>
+      <c r="AN9" s="23"/>
+      <c r="AO9" s="23"/>
+      <c r="AP9" s="23"/>
       <c r="AQ9" s="10"/>
       <c r="AR9" s="10"/>
       <c r="AS9" s="10"/>
@@ -1366,9 +1362,9 @@
       <c r="AK10" s="18"/>
       <c r="AL10" s="21"/>
       <c r="AM10" s="18"/>
-      <c r="AN10" s="25"/>
-      <c r="AO10" s="25"/>
-      <c r="AP10" s="25"/>
+      <c r="AN10" s="23"/>
+      <c r="AO10" s="23"/>
+      <c r="AP10" s="23"/>
       <c r="AQ10" s="10"/>
       <c r="AR10" s="10"/>
       <c r="AS10" s="10"/>
@@ -1430,9 +1426,9 @@
       <c r="AK11" s="18"/>
       <c r="AL11" s="21"/>
       <c r="AM11" s="18"/>
-      <c r="AN11" s="25"/>
-      <c r="AO11" s="25"/>
-      <c r="AP11" s="25"/>
+      <c r="AN11" s="23"/>
+      <c r="AO11" s="23"/>
+      <c r="AP11" s="23"/>
       <c r="AQ11" s="10"/>
       <c r="AR11" s="10"/>
       <c r="AS11" s="10"/>
@@ -1494,9 +1490,9 @@
       <c r="AK12" s="18"/>
       <c r="AL12" s="21"/>
       <c r="AM12" s="18"/>
-      <c r="AN12" s="25"/>
-      <c r="AO12" s="25"/>
-      <c r="AP12" s="25"/>
+      <c r="AN12" s="23"/>
+      <c r="AO12" s="23"/>
+      <c r="AP12" s="23"/>
       <c r="AQ12" s="10"/>
       <c r="AR12" s="10"/>
       <c r="AS12" s="10"/>
@@ -1558,9 +1554,9 @@
       <c r="AK13" s="18"/>
       <c r="AL13" s="21"/>
       <c r="AM13" s="18"/>
-      <c r="AN13" s="25"/>
-      <c r="AO13" s="25"/>
-      <c r="AP13" s="25"/>
+      <c r="AN13" s="23"/>
+      <c r="AO13" s="23"/>
+      <c r="AP13" s="23"/>
       <c r="AQ13" s="10"/>
       <c r="AR13" s="10"/>
       <c r="AS13" s="10"/>
@@ -1622,9 +1618,9 @@
       <c r="AK14" s="18"/>
       <c r="AL14" s="21"/>
       <c r="AM14" s="18"/>
-      <c r="AN14" s="25"/>
-      <c r="AO14" s="25"/>
-      <c r="AP14" s="25"/>
+      <c r="AN14" s="23"/>
+      <c r="AO14" s="23"/>
+      <c r="AP14" s="23"/>
       <c r="AQ14" s="10"/>
       <c r="AR14" s="10"/>
       <c r="AS14" s="10"/>
@@ -1686,9 +1682,9 @@
       <c r="AK15" s="18"/>
       <c r="AL15" s="21"/>
       <c r="AM15" s="18"/>
-      <c r="AN15" s="25"/>
-      <c r="AO15" s="25"/>
-      <c r="AP15" s="25"/>
+      <c r="AN15" s="23"/>
+      <c r="AO15" s="23"/>
+      <c r="AP15" s="23"/>
       <c r="AQ15" s="10"/>
       <c r="AR15" s="10"/>
       <c r="AS15" s="10"/>
@@ -1750,9 +1746,9 @@
       <c r="AK16" s="18"/>
       <c r="AL16" s="21"/>
       <c r="AM16" s="18"/>
-      <c r="AN16" s="25"/>
-      <c r="AO16" s="25"/>
-      <c r="AP16" s="25"/>
+      <c r="AN16" s="23"/>
+      <c r="AO16" s="23"/>
+      <c r="AP16" s="23"/>
       <c r="AQ16" s="10"/>
       <c r="AR16" s="10"/>
       <c r="AS16" s="10"/>
@@ -1814,9 +1810,9 @@
       <c r="AK17" s="18"/>
       <c r="AL17" s="21"/>
       <c r="AM17" s="18"/>
-      <c r="AN17" s="25"/>
-      <c r="AO17" s="25"/>
-      <c r="AP17" s="25"/>
+      <c r="AN17" s="23"/>
+      <c r="AO17" s="23"/>
+      <c r="AP17" s="23"/>
       <c r="AQ17" s="10"/>
       <c r="AR17" s="10"/>
       <c r="AS17" s="10"/>
@@ -1878,9 +1874,9 @@
       <c r="AK18" s="18"/>
       <c r="AL18" s="21"/>
       <c r="AM18" s="18"/>
-      <c r="AN18" s="25"/>
-      <c r="AO18" s="25"/>
-      <c r="AP18" s="25"/>
+      <c r="AN18" s="23"/>
+      <c r="AO18" s="23"/>
+      <c r="AP18" s="23"/>
       <c r="AQ18" s="10"/>
       <c r="AR18" s="10"/>
       <c r="AS18" s="10"/>
@@ -1942,9 +1938,9 @@
       <c r="AK19" s="18"/>
       <c r="AL19" s="21"/>
       <c r="AM19" s="18"/>
-      <c r="AN19" s="25"/>
-      <c r="AO19" s="25"/>
-      <c r="AP19" s="25"/>
+      <c r="AN19" s="23"/>
+      <c r="AO19" s="23"/>
+      <c r="AP19" s="23"/>
       <c r="AQ19" s="10"/>
       <c r="AR19" s="10"/>
       <c r="AS19" s="10"/>
@@ -2006,9 +2002,9 @@
       <c r="AK20" s="18"/>
       <c r="AL20" s="21"/>
       <c r="AM20" s="18"/>
-      <c r="AN20" s="25"/>
-      <c r="AO20" s="25"/>
-      <c r="AP20" s="25"/>
+      <c r="AN20" s="23"/>
+      <c r="AO20" s="23"/>
+      <c r="AP20" s="23"/>
       <c r="AQ20" s="10"/>
       <c r="AR20" s="10"/>
       <c r="AS20" s="10"/>
@@ -2070,9 +2066,9 @@
       <c r="AK21" s="18"/>
       <c r="AL21" s="21"/>
       <c r="AM21" s="18"/>
-      <c r="AN21" s="25"/>
-      <c r="AO21" s="25"/>
-      <c r="AP21" s="25"/>
+      <c r="AN21" s="23"/>
+      <c r="AO21" s="23"/>
+      <c r="AP21" s="23"/>
       <c r="AQ21" s="10"/>
       <c r="AR21" s="10"/>
       <c r="AS21" s="10"/>
@@ -2134,9 +2130,9 @@
       <c r="AK22" s="18"/>
       <c r="AL22" s="21"/>
       <c r="AM22" s="18"/>
-      <c r="AN22" s="25"/>
-      <c r="AO22" s="25"/>
-      <c r="AP22" s="25"/>
+      <c r="AN22" s="23"/>
+      <c r="AO22" s="23"/>
+      <c r="AP22" s="23"/>
       <c r="AQ22" s="10"/>
       <c r="AR22" s="10"/>
       <c r="AS22" s="10"/>
@@ -2198,9 +2194,9 @@
       <c r="AK23" s="18"/>
       <c r="AL23" s="21"/>
       <c r="AM23" s="18"/>
-      <c r="AN23" s="25"/>
-      <c r="AO23" s="25"/>
-      <c r="AP23" s="25"/>
+      <c r="AN23" s="23"/>
+      <c r="AO23" s="23"/>
+      <c r="AP23" s="23"/>
       <c r="AQ23" s="10"/>
       <c r="AR23" s="10"/>
       <c r="AS23" s="10"/>
@@ -2262,9 +2258,9 @@
       <c r="AK24" s="18"/>
       <c r="AL24" s="21"/>
       <c r="AM24" s="18"/>
-      <c r="AN24" s="25"/>
-      <c r="AO24" s="25"/>
-      <c r="AP24" s="25"/>
+      <c r="AN24" s="23"/>
+      <c r="AO24" s="23"/>
+      <c r="AP24" s="23"/>
       <c r="AQ24" s="10"/>
       <c r="AR24" s="10"/>
       <c r="AS24" s="10"/>
@@ -2326,9 +2322,9 @@
       <c r="AK25" s="18"/>
       <c r="AL25" s="21"/>
       <c r="AM25" s="18"/>
-      <c r="AN25" s="25"/>
-      <c r="AO25" s="25"/>
-      <c r="AP25" s="25"/>
+      <c r="AN25" s="23"/>
+      <c r="AO25" s="23"/>
+      <c r="AP25" s="23"/>
       <c r="AQ25" s="10"/>
       <c r="AR25" s="10"/>
       <c r="AS25" s="10"/>
@@ -2390,9 +2386,9 @@
       <c r="AK26" s="18"/>
       <c r="AL26" s="21"/>
       <c r="AM26" s="18"/>
-      <c r="AN26" s="25"/>
-      <c r="AO26" s="25"/>
-      <c r="AP26" s="25"/>
+      <c r="AN26" s="23"/>
+      <c r="AO26" s="23"/>
+      <c r="AP26" s="23"/>
       <c r="AQ26" s="10"/>
       <c r="AR26" s="10"/>
       <c r="AS26" s="10"/>
@@ -2454,9 +2450,9 @@
       <c r="AK27" s="18"/>
       <c r="AL27" s="21"/>
       <c r="AM27" s="18"/>
-      <c r="AN27" s="25"/>
-      <c r="AO27" s="25"/>
-      <c r="AP27" s="25"/>
+      <c r="AN27" s="23"/>
+      <c r="AO27" s="23"/>
+      <c r="AP27" s="23"/>
       <c r="AQ27" s="10"/>
       <c r="AR27" s="10"/>
       <c r="AS27" s="10"/>
@@ -2518,9 +2514,9 @@
       <c r="AK28" s="18"/>
       <c r="AL28" s="21"/>
       <c r="AM28" s="18"/>
-      <c r="AN28" s="25"/>
-      <c r="AO28" s="25"/>
-      <c r="AP28" s="25"/>
+      <c r="AN28" s="23"/>
+      <c r="AO28" s="23"/>
+      <c r="AP28" s="23"/>
       <c r="AQ28" s="10"/>
       <c r="AR28" s="10"/>
       <c r="AS28" s="10"/>
@@ -2582,9 +2578,9 @@
       <c r="AK29" s="18"/>
       <c r="AL29" s="21"/>
       <c r="AM29" s="18"/>
-      <c r="AN29" s="25"/>
-      <c r="AO29" s="25"/>
-      <c r="AP29" s="25"/>
+      <c r="AN29" s="23"/>
+      <c r="AO29" s="23"/>
+      <c r="AP29" s="23"/>
       <c r="AQ29" s="10"/>
       <c r="AR29" s="10"/>
       <c r="AS29" s="10"/>
@@ -2646,9 +2642,9 @@
       <c r="AK30" s="18"/>
       <c r="AL30" s="21"/>
       <c r="AM30" s="18"/>
-      <c r="AN30" s="25"/>
-      <c r="AO30" s="25"/>
-      <c r="AP30" s="25"/>
+      <c r="AN30" s="23"/>
+      <c r="AO30" s="23"/>
+      <c r="AP30" s="23"/>
       <c r="AQ30" s="10"/>
       <c r="AR30" s="10"/>
       <c r="AS30" s="10"/>
@@ -2710,9 +2706,9 @@
       <c r="AK31" s="18"/>
       <c r="AL31" s="21"/>
       <c r="AM31" s="18"/>
-      <c r="AN31" s="25"/>
-      <c r="AO31" s="25"/>
-      <c r="AP31" s="25"/>
+      <c r="AN31" s="23"/>
+      <c r="AO31" s="23"/>
+      <c r="AP31" s="23"/>
       <c r="AQ31" s="10"/>
       <c r="AR31" s="10"/>
       <c r="AS31" s="10"/>
@@ -2774,9 +2770,9 @@
       <c r="AK32" s="18"/>
       <c r="AL32" s="21"/>
       <c r="AM32" s="18"/>
-      <c r="AN32" s="25"/>
-      <c r="AO32" s="25"/>
-      <c r="AP32" s="25"/>
+      <c r="AN32" s="23"/>
+      <c r="AO32" s="23"/>
+      <c r="AP32" s="23"/>
       <c r="AQ32" s="10"/>
       <c r="AR32" s="10"/>
       <c r="AS32" s="10"/>
@@ -2838,9 +2834,9 @@
       <c r="AK33" s="18"/>
       <c r="AL33" s="21"/>
       <c r="AM33" s="18"/>
-      <c r="AN33" s="25"/>
-      <c r="AO33" s="25"/>
-      <c r="AP33" s="25"/>
+      <c r="AN33" s="23"/>
+      <c r="AO33" s="23"/>
+      <c r="AP33" s="23"/>
       <c r="AQ33" s="10"/>
       <c r="AR33" s="10"/>
       <c r="AS33" s="10"/>
@@ -2902,9 +2898,9 @@
       <c r="AK34" s="18"/>
       <c r="AL34" s="21"/>
       <c r="AM34" s="18"/>
-      <c r="AN34" s="25"/>
-      <c r="AO34" s="25"/>
-      <c r="AP34" s="25"/>
+      <c r="AN34" s="23"/>
+      <c r="AO34" s="23"/>
+      <c r="AP34" s="23"/>
       <c r="AQ34" s="10"/>
       <c r="AR34" s="10"/>
       <c r="AS34" s="10"/>
@@ -2966,9 +2962,9 @@
       <c r="AK35" s="18"/>
       <c r="AL35" s="21"/>
       <c r="AM35" s="18"/>
-      <c r="AN35" s="25"/>
-      <c r="AO35" s="25"/>
-      <c r="AP35" s="25"/>
+      <c r="AN35" s="23"/>
+      <c r="AO35" s="23"/>
+      <c r="AP35" s="23"/>
       <c r="AQ35" s="10"/>
       <c r="AR35" s="10"/>
       <c r="AS35" s="10"/>
@@ -3030,9 +3026,9 @@
       <c r="AK36" s="18"/>
       <c r="AL36" s="21"/>
       <c r="AM36" s="18"/>
-      <c r="AN36" s="25"/>
-      <c r="AO36" s="25"/>
-      <c r="AP36" s="25"/>
+      <c r="AN36" s="23"/>
+      <c r="AO36" s="23"/>
+      <c r="AP36" s="23"/>
       <c r="AQ36" s="10"/>
       <c r="AR36" s="10"/>
       <c r="AS36" s="10"/>
@@ -3094,9 +3090,9 @@
       <c r="AK37" s="18"/>
       <c r="AL37" s="21"/>
       <c r="AM37" s="18"/>
-      <c r="AN37" s="25"/>
-      <c r="AO37" s="25"/>
-      <c r="AP37" s="25"/>
+      <c r="AN37" s="23"/>
+      <c r="AO37" s="23"/>
+      <c r="AP37" s="23"/>
       <c r="AQ37" s="10"/>
       <c r="AR37" s="10"/>
       <c r="AS37" s="10"/>
@@ -3158,9 +3154,9 @@
       <c r="AK38" s="18"/>
       <c r="AL38" s="21"/>
       <c r="AM38" s="18"/>
-      <c r="AN38" s="25"/>
-      <c r="AO38" s="25"/>
-      <c r="AP38" s="25"/>
+      <c r="AN38" s="23"/>
+      <c r="AO38" s="23"/>
+      <c r="AP38" s="23"/>
       <c r="AQ38" s="10"/>
       <c r="AR38" s="10"/>
       <c r="AS38" s="10"/>
@@ -3222,9 +3218,9 @@
       <c r="AK39" s="18"/>
       <c r="AL39" s="21"/>
       <c r="AM39" s="18"/>
-      <c r="AN39" s="25"/>
-      <c r="AO39" s="25"/>
-      <c r="AP39" s="25"/>
+      <c r="AN39" s="23"/>
+      <c r="AO39" s="23"/>
+      <c r="AP39" s="23"/>
       <c r="AQ39" s="10"/>
       <c r="AR39" s="10"/>
       <c r="AS39" s="10"/>
@@ -3286,9 +3282,9 @@
       <c r="AK40" s="18"/>
       <c r="AL40" s="21"/>
       <c r="AM40" s="18"/>
-      <c r="AN40" s="25"/>
-      <c r="AO40" s="25"/>
-      <c r="AP40" s="25"/>
+      <c r="AN40" s="23"/>
+      <c r="AO40" s="23"/>
+      <c r="AP40" s="23"/>
       <c r="AQ40" s="10"/>
       <c r="AR40" s="10"/>
       <c r="AS40" s="10"/>
@@ -3350,9 +3346,9 @@
       <c r="AK41" s="18"/>
       <c r="AL41" s="21"/>
       <c r="AM41" s="18"/>
-      <c r="AN41" s="25"/>
-      <c r="AO41" s="25"/>
-      <c r="AP41" s="25"/>
+      <c r="AN41" s="23"/>
+      <c r="AO41" s="23"/>
+      <c r="AP41" s="23"/>
       <c r="AQ41" s="10"/>
       <c r="AR41" s="10"/>
       <c r="AS41" s="10"/>
@@ -3414,9 +3410,9 @@
       <c r="AK42" s="18"/>
       <c r="AL42" s="21"/>
       <c r="AM42" s="18"/>
-      <c r="AN42" s="25"/>
-      <c r="AO42" s="25"/>
-      <c r="AP42" s="25"/>
+      <c r="AN42" s="23"/>
+      <c r="AO42" s="23"/>
+      <c r="AP42" s="23"/>
       <c r="AQ42" s="10"/>
       <c r="AR42" s="10"/>
       <c r="AS42" s="10"/>
@@ -3478,9 +3474,9 @@
       <c r="AK43" s="18"/>
       <c r="AL43" s="21"/>
       <c r="AM43" s="18"/>
-      <c r="AN43" s="25"/>
-      <c r="AO43" s="25"/>
-      <c r="AP43" s="25"/>
+      <c r="AN43" s="23"/>
+      <c r="AO43" s="23"/>
+      <c r="AP43" s="23"/>
       <c r="AQ43" s="10"/>
       <c r="AR43" s="10"/>
       <c r="AS43" s="10"/>
@@ -3542,9 +3538,9 @@
       <c r="AK44" s="18"/>
       <c r="AL44" s="21"/>
       <c r="AM44" s="18"/>
-      <c r="AN44" s="25"/>
-      <c r="AO44" s="25"/>
-      <c r="AP44" s="25"/>
+      <c r="AN44" s="23"/>
+      <c r="AO44" s="23"/>
+      <c r="AP44" s="23"/>
       <c r="AQ44" s="10"/>
       <c r="AR44" s="10"/>
       <c r="AS44" s="10"/>
@@ -3606,9 +3602,9 @@
       <c r="AK45" s="18"/>
       <c r="AL45" s="21"/>
       <c r="AM45" s="18"/>
-      <c r="AN45" s="25"/>
-      <c r="AO45" s="25"/>
-      <c r="AP45" s="25"/>
+      <c r="AN45" s="23"/>
+      <c r="AO45" s="23"/>
+      <c r="AP45" s="23"/>
       <c r="AQ45" s="10"/>
       <c r="AR45" s="10"/>
       <c r="AS45" s="10"/>
@@ -3670,9 +3666,9 @@
       <c r="AK46" s="18"/>
       <c r="AL46" s="21"/>
       <c r="AM46" s="18"/>
-      <c r="AN46" s="25"/>
-      <c r="AO46" s="25"/>
-      <c r="AP46" s="25"/>
+      <c r="AN46" s="23"/>
+      <c r="AO46" s="23"/>
+      <c r="AP46" s="23"/>
       <c r="AQ46" s="10"/>
       <c r="AR46" s="10"/>
       <c r="AS46" s="10"/>
@@ -3734,9 +3730,9 @@
       <c r="AK47" s="18"/>
       <c r="AL47" s="21"/>
       <c r="AM47" s="18"/>
-      <c r="AN47" s="25"/>
-      <c r="AO47" s="25"/>
-      <c r="AP47" s="25"/>
+      <c r="AN47" s="23"/>
+      <c r="AO47" s="23"/>
+      <c r="AP47" s="23"/>
       <c r="AQ47" s="10"/>
       <c r="AR47" s="10"/>
       <c r="AS47" s="10"/>
@@ -3798,9 +3794,9 @@
       <c r="AK48" s="18"/>
       <c r="AL48" s="21"/>
       <c r="AM48" s="18"/>
-      <c r="AN48" s="25"/>
-      <c r="AO48" s="25"/>
-      <c r="AP48" s="25"/>
+      <c r="AN48" s="23"/>
+      <c r="AO48" s="23"/>
+      <c r="AP48" s="23"/>
       <c r="AQ48" s="10"/>
       <c r="AR48" s="10"/>
       <c r="AS48" s="10"/>
@@ -3862,9 +3858,9 @@
       <c r="AK49" s="18"/>
       <c r="AL49" s="21"/>
       <c r="AM49" s="18"/>
-      <c r="AN49" s="25"/>
-      <c r="AO49" s="25"/>
-      <c r="AP49" s="25"/>
+      <c r="AN49" s="23"/>
+      <c r="AO49" s="23"/>
+      <c r="AP49" s="23"/>
       <c r="AQ49" s="10"/>
       <c r="AR49" s="10"/>
       <c r="AS49" s="10"/>
@@ -3926,9 +3922,9 @@
       <c r="AK50" s="18"/>
       <c r="AL50" s="21"/>
       <c r="AM50" s="18"/>
-      <c r="AN50" s="25"/>
-      <c r="AO50" s="25"/>
-      <c r="AP50" s="25"/>
+      <c r="AN50" s="23"/>
+      <c r="AO50" s="23"/>
+      <c r="AP50" s="23"/>
       <c r="AQ50" s="10"/>
       <c r="AR50" s="10"/>
       <c r="AS50" s="10"/>
@@ -3990,9 +3986,9 @@
       <c r="AK51" s="18"/>
       <c r="AL51" s="21"/>
       <c r="AM51" s="18"/>
-      <c r="AN51" s="25"/>
-      <c r="AO51" s="25"/>
-      <c r="AP51" s="25"/>
+      <c r="AN51" s="23"/>
+      <c r="AO51" s="23"/>
+      <c r="AP51" s="23"/>
       <c r="AQ51" s="10"/>
       <c r="AR51" s="10"/>
       <c r="AS51" s="10"/>
@@ -4054,9 +4050,9 @@
       <c r="AK52" s="18"/>
       <c r="AL52" s="21"/>
       <c r="AM52" s="18"/>
-      <c r="AN52" s="25"/>
-      <c r="AO52" s="25"/>
-      <c r="AP52" s="25"/>
+      <c r="AN52" s="23"/>
+      <c r="AO52" s="23"/>
+      <c r="AP52" s="23"/>
       <c r="AQ52" s="10"/>
       <c r="AR52" s="10"/>
       <c r="AS52" s="10"/>
@@ -4118,9 +4114,9 @@
       <c r="AK53" s="18"/>
       <c r="AL53" s="21"/>
       <c r="AM53" s="18"/>
-      <c r="AN53" s="25"/>
-      <c r="AO53" s="25"/>
-      <c r="AP53" s="25"/>
+      <c r="AN53" s="23"/>
+      <c r="AO53" s="23"/>
+      <c r="AP53" s="23"/>
       <c r="AQ53" s="10"/>
       <c r="AR53" s="10"/>
       <c r="AS53" s="10"/>
@@ -4182,9 +4178,9 @@
       <c r="AK54" s="18"/>
       <c r="AL54" s="21"/>
       <c r="AM54" s="18"/>
-      <c r="AN54" s="25"/>
-      <c r="AO54" s="25"/>
-      <c r="AP54" s="25"/>
+      <c r="AN54" s="23"/>
+      <c r="AO54" s="23"/>
+      <c r="AP54" s="23"/>
       <c r="AQ54" s="10"/>
       <c r="AR54" s="10"/>
       <c r="AS54" s="10"/>
@@ -4246,9 +4242,9 @@
       <c r="AK55" s="18"/>
       <c r="AL55" s="21"/>
       <c r="AM55" s="18"/>
-      <c r="AN55" s="25"/>
-      <c r="AO55" s="25"/>
-      <c r="AP55" s="25"/>
+      <c r="AN55" s="23"/>
+      <c r="AO55" s="23"/>
+      <c r="AP55" s="23"/>
       <c r="AQ55" s="10"/>
       <c r="AR55" s="10"/>
       <c r="AS55" s="10"/>
@@ -4310,9 +4306,9 @@
       <c r="AK56" s="18"/>
       <c r="AL56" s="21"/>
       <c r="AM56" s="18"/>
-      <c r="AN56" s="25"/>
-      <c r="AO56" s="25"/>
-      <c r="AP56" s="25"/>
+      <c r="AN56" s="23"/>
+      <c r="AO56" s="23"/>
+      <c r="AP56" s="23"/>
       <c r="AQ56" s="10"/>
       <c r="AR56" s="10"/>
       <c r="AS56" s="10"/>
@@ -4374,9 +4370,9 @@
       <c r="AK57" s="18"/>
       <c r="AL57" s="21"/>
       <c r="AM57" s="18"/>
-      <c r="AN57" s="25"/>
-      <c r="AO57" s="25"/>
-      <c r="AP57" s="25"/>
+      <c r="AN57" s="23"/>
+      <c r="AO57" s="23"/>
+      <c r="AP57" s="23"/>
       <c r="AQ57" s="10"/>
       <c r="AR57" s="10"/>
       <c r="AS57" s="10"/>
@@ -4438,9 +4434,9 @@
       <c r="AK58" s="18"/>
       <c r="AL58" s="21"/>
       <c r="AM58" s="18"/>
-      <c r="AN58" s="25"/>
-      <c r="AO58" s="25"/>
-      <c r="AP58" s="25"/>
+      <c r="AN58" s="23"/>
+      <c r="AO58" s="23"/>
+      <c r="AP58" s="23"/>
       <c r="AQ58" s="10"/>
       <c r="AR58" s="10"/>
       <c r="AS58" s="10"/>
@@ -4502,9 +4498,9 @@
       <c r="AK59" s="18"/>
       <c r="AL59" s="21"/>
       <c r="AM59" s="18"/>
-      <c r="AN59" s="25"/>
-      <c r="AO59" s="25"/>
-      <c r="AP59" s="25"/>
+      <c r="AN59" s="23"/>
+      <c r="AO59" s="23"/>
+      <c r="AP59" s="23"/>
       <c r="AQ59" s="10"/>
       <c r="AR59" s="10"/>
       <c r="AS59" s="10"/>
@@ -4566,9 +4562,9 @@
       <c r="AK60" s="18"/>
       <c r="AL60" s="21"/>
       <c r="AM60" s="18"/>
-      <c r="AN60" s="25"/>
-      <c r="AO60" s="25"/>
-      <c r="AP60" s="25"/>
+      <c r="AN60" s="23"/>
+      <c r="AO60" s="23"/>
+      <c r="AP60" s="23"/>
       <c r="AQ60" s="10"/>
       <c r="AR60" s="10"/>
       <c r="AS60" s="10"/>
@@ -4630,9 +4626,9 @@
       <c r="AK61" s="18"/>
       <c r="AL61" s="21"/>
       <c r="AM61" s="18"/>
-      <c r="AN61" s="25"/>
-      <c r="AO61" s="25"/>
-      <c r="AP61" s="25"/>
+      <c r="AN61" s="23"/>
+      <c r="AO61" s="23"/>
+      <c r="AP61" s="23"/>
       <c r="AQ61" s="10"/>
       <c r="AR61" s="10"/>
       <c r="AS61" s="10"/>
@@ -4694,9 +4690,9 @@
       <c r="AK62" s="18"/>
       <c r="AL62" s="21"/>
       <c r="AM62" s="18"/>
-      <c r="AN62" s="25"/>
-      <c r="AO62" s="25"/>
-      <c r="AP62" s="25"/>
+      <c r="AN62" s="23"/>
+      <c r="AO62" s="23"/>
+      <c r="AP62" s="23"/>
       <c r="AQ62" s="10"/>
       <c r="AR62" s="10"/>
       <c r="AS62" s="10"/>
@@ -4758,9 +4754,9 @@
       <c r="AK63" s="18"/>
       <c r="AL63" s="21"/>
       <c r="AM63" s="18"/>
-      <c r="AN63" s="25"/>
-      <c r="AO63" s="25"/>
-      <c r="AP63" s="25"/>
+      <c r="AN63" s="23"/>
+      <c r="AO63" s="23"/>
+      <c r="AP63" s="23"/>
       <c r="AQ63" s="10"/>
       <c r="AR63" s="10"/>
       <c r="AS63" s="10"/>
@@ -4822,9 +4818,9 @@
       <c r="AK64" s="18"/>
       <c r="AL64" s="21"/>
       <c r="AM64" s="18"/>
-      <c r="AN64" s="25"/>
-      <c r="AO64" s="25"/>
-      <c r="AP64" s="25"/>
+      <c r="AN64" s="23"/>
+      <c r="AO64" s="23"/>
+      <c r="AP64" s="23"/>
       <c r="AQ64" s="10"/>
       <c r="AR64" s="10"/>
       <c r="AS64" s="10"/>
@@ -4886,9 +4882,9 @@
       <c r="AK65" s="18"/>
       <c r="AL65" s="21"/>
       <c r="AM65" s="18"/>
-      <c r="AN65" s="25"/>
-      <c r="AO65" s="25"/>
-      <c r="AP65" s="25"/>
+      <c r="AN65" s="23"/>
+      <c r="AO65" s="23"/>
+      <c r="AP65" s="23"/>
       <c r="AQ65" s="10"/>
       <c r="AR65" s="10"/>
       <c r="AS65" s="10"/>
@@ -4950,9 +4946,9 @@
       <c r="AK66" s="18"/>
       <c r="AL66" s="21"/>
       <c r="AM66" s="18"/>
-      <c r="AN66" s="25"/>
-      <c r="AO66" s="25"/>
-      <c r="AP66" s="25"/>
+      <c r="AN66" s="23"/>
+      <c r="AO66" s="23"/>
+      <c r="AP66" s="23"/>
       <c r="AQ66" s="10"/>
       <c r="AR66" s="10"/>
       <c r="AS66" s="10"/>
@@ -5014,9 +5010,9 @@
       <c r="AK67" s="18"/>
       <c r="AL67" s="21"/>
       <c r="AM67" s="18"/>
-      <c r="AN67" s="25"/>
-      <c r="AO67" s="25"/>
-      <c r="AP67" s="25"/>
+      <c r="AN67" s="23"/>
+      <c r="AO67" s="23"/>
+      <c r="AP67" s="23"/>
       <c r="AQ67" s="10"/>
       <c r="AR67" s="10"/>
       <c r="AS67" s="10"/>
@@ -5078,9 +5074,9 @@
       <c r="AK68" s="18"/>
       <c r="AL68" s="21"/>
       <c r="AM68" s="18"/>
-      <c r="AN68" s="25"/>
-      <c r="AO68" s="25"/>
-      <c r="AP68" s="25"/>
+      <c r="AN68" s="23"/>
+      <c r="AO68" s="23"/>
+      <c r="AP68" s="23"/>
       <c r="AQ68" s="10"/>
       <c r="AR68" s="10"/>
       <c r="AS68" s="10"/>
@@ -5142,9 +5138,9 @@
       <c r="AK69" s="18"/>
       <c r="AL69" s="21"/>
       <c r="AM69" s="18"/>
-      <c r="AN69" s="25"/>
-      <c r="AO69" s="25"/>
-      <c r="AP69" s="25"/>
+      <c r="AN69" s="23"/>
+      <c r="AO69" s="23"/>
+      <c r="AP69" s="23"/>
       <c r="AQ69" s="10"/>
       <c r="AR69" s="10"/>
       <c r="AS69" s="10"/>
@@ -5206,9 +5202,9 @@
       <c r="AK70" s="18"/>
       <c r="AL70" s="21"/>
       <c r="AM70" s="18"/>
-      <c r="AN70" s="25"/>
-      <c r="AO70" s="25"/>
-      <c r="AP70" s="25"/>
+      <c r="AN70" s="23"/>
+      <c r="AO70" s="23"/>
+      <c r="AP70" s="23"/>
       <c r="AQ70" s="10"/>
       <c r="AR70" s="10"/>
       <c r="AS70" s="10"/>
@@ -5270,9 +5266,9 @@
       <c r="AK71" s="18"/>
       <c r="AL71" s="21"/>
       <c r="AM71" s="18"/>
-      <c r="AN71" s="25"/>
-      <c r="AO71" s="25"/>
-      <c r="AP71" s="25"/>
+      <c r="AN71" s="23"/>
+      <c r="AO71" s="23"/>
+      <c r="AP71" s="23"/>
       <c r="AQ71" s="10"/>
       <c r="AR71" s="10"/>
       <c r="AS71" s="10"/>
@@ -5334,9 +5330,9 @@
       <c r="AK72" s="18"/>
       <c r="AL72" s="21"/>
       <c r="AM72" s="18"/>
-      <c r="AN72" s="25"/>
-      <c r="AO72" s="25"/>
-      <c r="AP72" s="25"/>
+      <c r="AN72" s="23"/>
+      <c r="AO72" s="23"/>
+      <c r="AP72" s="23"/>
       <c r="AQ72" s="10"/>
       <c r="AR72" s="10"/>
       <c r="AS72" s="10"/>
@@ -5398,9 +5394,9 @@
       <c r="AK73" s="18"/>
       <c r="AL73" s="21"/>
       <c r="AM73" s="18"/>
-      <c r="AN73" s="25"/>
-      <c r="AO73" s="25"/>
-      <c r="AP73" s="25"/>
+      <c r="AN73" s="23"/>
+      <c r="AO73" s="23"/>
+      <c r="AP73" s="23"/>
       <c r="AQ73" s="10"/>
       <c r="AR73" s="10"/>
       <c r="AS73" s="10"/>
@@ -5462,9 +5458,9 @@
       <c r="AK74" s="18"/>
       <c r="AL74" s="21"/>
       <c r="AM74" s="18"/>
-      <c r="AN74" s="25"/>
-      <c r="AO74" s="25"/>
-      <c r="AP74" s="25"/>
+      <c r="AN74" s="23"/>
+      <c r="AO74" s="23"/>
+      <c r="AP74" s="23"/>
       <c r="AQ74" s="10"/>
       <c r="AR74" s="10"/>
       <c r="AS74" s="10"/>
@@ -5526,9 +5522,9 @@
       <c r="AK75" s="18"/>
       <c r="AL75" s="21"/>
       <c r="AM75" s="18"/>
-      <c r="AN75" s="25"/>
-      <c r="AO75" s="25"/>
-      <c r="AP75" s="25"/>
+      <c r="AN75" s="23"/>
+      <c r="AO75" s="23"/>
+      <c r="AP75" s="23"/>
       <c r="AQ75" s="10"/>
       <c r="AR75" s="10"/>
       <c r="AS75" s="10"/>
@@ -5590,9 +5586,9 @@
       <c r="AK76" s="18"/>
       <c r="AL76" s="21"/>
       <c r="AM76" s="18"/>
-      <c r="AN76" s="25"/>
-      <c r="AO76" s="25"/>
-      <c r="AP76" s="25"/>
+      <c r="AN76" s="23"/>
+      <c r="AO76" s="23"/>
+      <c r="AP76" s="23"/>
       <c r="AQ76" s="10"/>
       <c r="AR76" s="10"/>
       <c r="AS76" s="10"/>
@@ -5654,9 +5650,9 @@
       <c r="AK77" s="18"/>
       <c r="AL77" s="21"/>
       <c r="AM77" s="18"/>
-      <c r="AN77" s="25"/>
-      <c r="AO77" s="25"/>
-      <c r="AP77" s="25"/>
+      <c r="AN77" s="23"/>
+      <c r="AO77" s="23"/>
+      <c r="AP77" s="23"/>
       <c r="AQ77" s="10"/>
       <c r="AR77" s="10"/>
       <c r="AS77" s="10"/>
@@ -5718,9 +5714,9 @@
       <c r="AK78" s="18"/>
       <c r="AL78" s="21"/>
       <c r="AM78" s="18"/>
-      <c r="AN78" s="25"/>
-      <c r="AO78" s="25"/>
-      <c r="AP78" s="25"/>
+      <c r="AN78" s="23"/>
+      <c r="AO78" s="23"/>
+      <c r="AP78" s="23"/>
       <c r="AQ78" s="10"/>
       <c r="AR78" s="10"/>
       <c r="AS78" s="10"/>
@@ -5782,9 +5778,9 @@
       <c r="AK79" s="18"/>
       <c r="AL79" s="21"/>
       <c r="AM79" s="18"/>
-      <c r="AN79" s="25"/>
-      <c r="AO79" s="25"/>
-      <c r="AP79" s="25"/>
+      <c r="AN79" s="23"/>
+      <c r="AO79" s="23"/>
+      <c r="AP79" s="23"/>
       <c r="AQ79" s="10"/>
       <c r="AR79" s="10"/>
       <c r="AS79" s="10"/>
@@ -5846,9 +5842,9 @@
       <c r="AK80" s="18"/>
       <c r="AL80" s="21"/>
       <c r="AM80" s="18"/>
-      <c r="AN80" s="25"/>
-      <c r="AO80" s="25"/>
-      <c r="AP80" s="25"/>
+      <c r="AN80" s="23"/>
+      <c r="AO80" s="23"/>
+      <c r="AP80" s="23"/>
       <c r="AQ80" s="10"/>
       <c r="AR80" s="10"/>
       <c r="AS80" s="10"/>
@@ -5910,9 +5906,9 @@
       <c r="AK81" s="18"/>
       <c r="AL81" s="21"/>
       <c r="AM81" s="18"/>
-      <c r="AN81" s="25"/>
-      <c r="AO81" s="25"/>
-      <c r="AP81" s="25"/>
+      <c r="AN81" s="23"/>
+      <c r="AO81" s="23"/>
+      <c r="AP81" s="23"/>
       <c r="AQ81" s="10"/>
       <c r="AR81" s="10"/>
       <c r="AS81" s="10"/>
@@ -5974,9 +5970,9 @@
       <c r="AK82" s="18"/>
       <c r="AL82" s="21"/>
       <c r="AM82" s="18"/>
-      <c r="AN82" s="25"/>
-      <c r="AO82" s="25"/>
-      <c r="AP82" s="25"/>
+      <c r="AN82" s="23"/>
+      <c r="AO82" s="23"/>
+      <c r="AP82" s="23"/>
       <c r="AQ82" s="10"/>
       <c r="AR82" s="10"/>
       <c r="AS82" s="10"/>
@@ -6038,9 +6034,9 @@
       <c r="AK83" s="18"/>
       <c r="AL83" s="21"/>
       <c r="AM83" s="18"/>
-      <c r="AN83" s="25"/>
-      <c r="AO83" s="25"/>
-      <c r="AP83" s="25"/>
+      <c r="AN83" s="23"/>
+      <c r="AO83" s="23"/>
+      <c r="AP83" s="23"/>
       <c r="AQ83" s="10"/>
       <c r="AR83" s="10"/>
       <c r="AS83" s="10"/>
@@ -6102,9 +6098,9 @@
       <c r="AK84" s="18"/>
       <c r="AL84" s="21"/>
       <c r="AM84" s="18"/>
-      <c r="AN84" s="25"/>
-      <c r="AO84" s="25"/>
-      <c r="AP84" s="25"/>
+      <c r="AN84" s="23"/>
+      <c r="AO84" s="23"/>
+      <c r="AP84" s="23"/>
       <c r="AQ84" s="10"/>
       <c r="AR84" s="10"/>
       <c r="AS84" s="10"/>
@@ -6166,9 +6162,9 @@
       <c r="AK85" s="18"/>
       <c r="AL85" s="21"/>
       <c r="AM85" s="18"/>
-      <c r="AN85" s="25"/>
-      <c r="AO85" s="25"/>
-      <c r="AP85" s="25"/>
+      <c r="AN85" s="23"/>
+      <c r="AO85" s="23"/>
+      <c r="AP85" s="23"/>
       <c r="AQ85" s="10"/>
       <c r="AR85" s="10"/>
       <c r="AS85" s="10"/>
@@ -6230,9 +6226,9 @@
       <c r="AK86" s="18"/>
       <c r="AL86" s="21"/>
       <c r="AM86" s="18"/>
-      <c r="AN86" s="25"/>
-      <c r="AO86" s="25"/>
-      <c r="AP86" s="25"/>
+      <c r="AN86" s="23"/>
+      <c r="AO86" s="23"/>
+      <c r="AP86" s="23"/>
       <c r="AQ86" s="10"/>
       <c r="AR86" s="10"/>
       <c r="AS86" s="10"/>
@@ -6294,9 +6290,9 @@
       <c r="AK87" s="18"/>
       <c r="AL87" s="21"/>
       <c r="AM87" s="18"/>
-      <c r="AN87" s="25"/>
-      <c r="AO87" s="25"/>
-      <c r="AP87" s="25"/>
+      <c r="AN87" s="23"/>
+      <c r="AO87" s="23"/>
+      <c r="AP87" s="23"/>
       <c r="AQ87" s="10"/>
       <c r="AR87" s="10"/>
       <c r="AS87" s="10"/>
@@ -6358,9 +6354,9 @@
       <c r="AK88" s="18"/>
       <c r="AL88" s="21"/>
       <c r="AM88" s="18"/>
-      <c r="AN88" s="25"/>
-      <c r="AO88" s="25"/>
-      <c r="AP88" s="25"/>
+      <c r="AN88" s="23"/>
+      <c r="AO88" s="23"/>
+      <c r="AP88" s="23"/>
       <c r="AQ88" s="10"/>
       <c r="AR88" s="10"/>
       <c r="AS88" s="10"/>
@@ -6422,9 +6418,9 @@
       <c r="AK89" s="18"/>
       <c r="AL89" s="21"/>
       <c r="AM89" s="18"/>
-      <c r="AN89" s="25"/>
-      <c r="AO89" s="25"/>
-      <c r="AP89" s="25"/>
+      <c r="AN89" s="23"/>
+      <c r="AO89" s="23"/>
+      <c r="AP89" s="23"/>
       <c r="AQ89" s="10"/>
       <c r="AR89" s="10"/>
       <c r="AS89" s="10"/>
@@ -6486,9 +6482,9 @@
       <c r="AK90" s="18"/>
       <c r="AL90" s="21"/>
       <c r="AM90" s="18"/>
-      <c r="AN90" s="25"/>
-      <c r="AO90" s="25"/>
-      <c r="AP90" s="25"/>
+      <c r="AN90" s="23"/>
+      <c r="AO90" s="23"/>
+      <c r="AP90" s="23"/>
       <c r="AQ90" s="10"/>
       <c r="AR90" s="10"/>
       <c r="AS90" s="10"/>
@@ -6550,9 +6546,9 @@
       <c r="AK91" s="18"/>
       <c r="AL91" s="21"/>
       <c r="AM91" s="18"/>
-      <c r="AN91" s="25"/>
-      <c r="AO91" s="25"/>
-      <c r="AP91" s="25"/>
+      <c r="AN91" s="23"/>
+      <c r="AO91" s="23"/>
+      <c r="AP91" s="23"/>
       <c r="AQ91" s="10"/>
       <c r="AR91" s="10"/>
       <c r="AS91" s="10"/>
@@ -6614,9 +6610,9 @@
       <c r="AK92" s="18"/>
       <c r="AL92" s="21"/>
       <c r="AM92" s="18"/>
-      <c r="AN92" s="25"/>
-      <c r="AO92" s="25"/>
-      <c r="AP92" s="25"/>
+      <c r="AN92" s="23"/>
+      <c r="AO92" s="23"/>
+      <c r="AP92" s="23"/>
       <c r="AQ92" s="10"/>
       <c r="AR92" s="10"/>
       <c r="AS92" s="10"/>
@@ -6678,9 +6674,9 @@
       <c r="AK93" s="18"/>
       <c r="AL93" s="21"/>
       <c r="AM93" s="18"/>
-      <c r="AN93" s="25"/>
-      <c r="AO93" s="25"/>
-      <c r="AP93" s="25"/>
+      <c r="AN93" s="23"/>
+      <c r="AO93" s="23"/>
+      <c r="AP93" s="23"/>
       <c r="AQ93" s="10"/>
       <c r="AR93" s="10"/>
       <c r="AS93" s="10"/>
@@ -6742,9 +6738,9 @@
       <c r="AK94" s="18"/>
       <c r="AL94" s="21"/>
       <c r="AM94" s="18"/>
-      <c r="AN94" s="25"/>
-      <c r="AO94" s="25"/>
-      <c r="AP94" s="25"/>
+      <c r="AN94" s="23"/>
+      <c r="AO94" s="23"/>
+      <c r="AP94" s="23"/>
       <c r="AQ94" s="10"/>
       <c r="AR94" s="10"/>
       <c r="AS94" s="10"/>
@@ -6806,9 +6802,9 @@
       <c r="AK95" s="18"/>
       <c r="AL95" s="21"/>
       <c r="AM95" s="18"/>
-      <c r="AN95" s="25"/>
-      <c r="AO95" s="25"/>
-      <c r="AP95" s="25"/>
+      <c r="AN95" s="23"/>
+      <c r="AO95" s="23"/>
+      <c r="AP95" s="23"/>
       <c r="AQ95" s="10"/>
       <c r="AR95" s="10"/>
       <c r="AS95" s="10"/>
@@ -6870,9 +6866,9 @@
       <c r="AK96" s="18"/>
       <c r="AL96" s="21"/>
       <c r="AM96" s="18"/>
-      <c r="AN96" s="25"/>
-      <c r="AO96" s="25"/>
-      <c r="AP96" s="25"/>
+      <c r="AN96" s="23"/>
+      <c r="AO96" s="23"/>
+      <c r="AP96" s="23"/>
       <c r="AQ96" s="10"/>
       <c r="AR96" s="10"/>
       <c r="AS96" s="10"/>
@@ -6934,9 +6930,9 @@
       <c r="AK97" s="18"/>
       <c r="AL97" s="21"/>
       <c r="AM97" s="18"/>
-      <c r="AN97" s="25"/>
-      <c r="AO97" s="25"/>
-      <c r="AP97" s="25"/>
+      <c r="AN97" s="23"/>
+      <c r="AO97" s="23"/>
+      <c r="AP97" s="23"/>
       <c r="AQ97" s="10"/>
       <c r="AR97" s="10"/>
       <c r="AS97" s="10"/>
@@ -6998,9 +6994,9 @@
       <c r="AK98" s="18"/>
       <c r="AL98" s="21"/>
       <c r="AM98" s="18"/>
-      <c r="AN98" s="25"/>
-      <c r="AO98" s="25"/>
-      <c r="AP98" s="25"/>
+      <c r="AN98" s="23"/>
+      <c r="AO98" s="23"/>
+      <c r="AP98" s="23"/>
       <c r="AQ98" s="10"/>
       <c r="AR98" s="10"/>
       <c r="AS98" s="10"/>
@@ -7062,9 +7058,9 @@
       <c r="AK99" s="18"/>
       <c r="AL99" s="21"/>
       <c r="AM99" s="18"/>
-      <c r="AN99" s="25"/>
-      <c r="AO99" s="25"/>
-      <c r="AP99" s="25"/>
+      <c r="AN99" s="23"/>
+      <c r="AO99" s="23"/>
+      <c r="AP99" s="23"/>
       <c r="AQ99" s="10"/>
       <c r="AR99" s="10"/>
       <c r="AS99" s="10"/>
@@ -7126,9 +7122,9 @@
       <c r="AK100" s="18"/>
       <c r="AL100" s="21"/>
       <c r="AM100" s="18"/>
-      <c r="AN100" s="25"/>
-      <c r="AO100" s="25"/>
-      <c r="AP100" s="25"/>
+      <c r="AN100" s="23"/>
+      <c r="AO100" s="23"/>
+      <c r="AP100" s="23"/>
       <c r="AQ100" s="10"/>
       <c r="AR100" s="10"/>
       <c r="AS100" s="10"/>
@@ -7190,9 +7186,9 @@
       <c r="AK101" s="18"/>
       <c r="AL101" s="21"/>
       <c r="AM101" s="18"/>
-      <c r="AN101" s="25"/>
-      <c r="AO101" s="25"/>
-      <c r="AP101" s="25"/>
+      <c r="AN101" s="23"/>
+      <c r="AO101" s="23"/>
+      <c r="AP101" s="23"/>
       <c r="AQ101" s="10"/>
       <c r="AR101" s="10"/>
       <c r="AS101" s="10"/>
@@ -7254,9 +7250,9 @@
       <c r="AK102" s="18"/>
       <c r="AL102" s="21"/>
       <c r="AM102" s="18"/>
-      <c r="AN102" s="25"/>
-      <c r="AO102" s="25"/>
-      <c r="AP102" s="25"/>
+      <c r="AN102" s="23"/>
+      <c r="AO102" s="23"/>
+      <c r="AP102" s="23"/>
       <c r="AQ102" s="10"/>
       <c r="AR102" s="10"/>
       <c r="AS102" s="10"/>
@@ -7318,9 +7314,9 @@
       <c r="AK103" s="18"/>
       <c r="AL103" s="21"/>
       <c r="AM103" s="18"/>
-      <c r="AN103" s="25"/>
-      <c r="AO103" s="25"/>
-      <c r="AP103" s="25"/>
+      <c r="AN103" s="23"/>
+      <c r="AO103" s="23"/>
+      <c r="AP103" s="23"/>
       <c r="AQ103" s="10"/>
       <c r="AR103" s="10"/>
       <c r="AS103" s="10"/>
@@ -7382,9 +7378,9 @@
       <c r="AK104" s="18"/>
       <c r="AL104" s="21"/>
       <c r="AM104" s="18"/>
-      <c r="AN104" s="25"/>
-      <c r="AO104" s="25"/>
-      <c r="AP104" s="25"/>
+      <c r="AN104" s="23"/>
+      <c r="AO104" s="23"/>
+      <c r="AP104" s="23"/>
       <c r="AQ104" s="10"/>
       <c r="AR104" s="10"/>
       <c r="AS104" s="10"/>
@@ -7446,9 +7442,9 @@
       <c r="AK105" s="18"/>
       <c r="AL105" s="21"/>
       <c r="AM105" s="18"/>
-      <c r="AN105" s="25"/>
-      <c r="AO105" s="25"/>
-      <c r="AP105" s="25"/>
+      <c r="AN105" s="23"/>
+      <c r="AO105" s="23"/>
+      <c r="AP105" s="23"/>
       <c r="AQ105" s="10"/>
       <c r="AR105" s="10"/>
       <c r="AS105" s="10"/>
@@ -7510,9 +7506,9 @@
       <c r="AK106" s="18"/>
       <c r="AL106" s="21"/>
       <c r="AM106" s="18"/>
-      <c r="AN106" s="25"/>
-      <c r="AO106" s="25"/>
-      <c r="AP106" s="25"/>
+      <c r="AN106" s="23"/>
+      <c r="AO106" s="23"/>
+      <c r="AP106" s="23"/>
       <c r="AQ106" s="10"/>
       <c r="AR106" s="10"/>
       <c r="AS106" s="10"/>
@@ -7574,9 +7570,9 @@
       <c r="AK107" s="18"/>
       <c r="AL107" s="21"/>
       <c r="AM107" s="18"/>
-      <c r="AN107" s="25"/>
-      <c r="AO107" s="25"/>
-      <c r="AP107" s="25"/>
+      <c r="AN107" s="23"/>
+      <c r="AO107" s="23"/>
+      <c r="AP107" s="23"/>
       <c r="AQ107" s="10"/>
       <c r="AR107" s="10"/>
       <c r="AS107" s="10"/>
@@ -7638,9 +7634,9 @@
       <c r="AK108" s="18"/>
       <c r="AL108" s="21"/>
       <c r="AM108" s="18"/>
-      <c r="AN108" s="25"/>
-      <c r="AO108" s="25"/>
-      <c r="AP108" s="25"/>
+      <c r="AN108" s="23"/>
+      <c r="AO108" s="23"/>
+      <c r="AP108" s="23"/>
       <c r="AQ108" s="10"/>
       <c r="AR108" s="10"/>
       <c r="AS108" s="10"/>
@@ -7702,9 +7698,9 @@
       <c r="AK109" s="18"/>
       <c r="AL109" s="21"/>
       <c r="AM109" s="18"/>
-      <c r="AN109" s="25"/>
-      <c r="AO109" s="25"/>
-      <c r="AP109" s="25"/>
+      <c r="AN109" s="23"/>
+      <c r="AO109" s="23"/>
+      <c r="AP109" s="23"/>
       <c r="AQ109" s="10"/>
       <c r="AR109" s="10"/>
       <c r="AS109" s="10"/>
@@ -7766,9 +7762,9 @@
       <c r="AK110" s="18"/>
       <c r="AL110" s="21"/>
       <c r="AM110" s="18"/>
-      <c r="AN110" s="25"/>
-      <c r="AO110" s="25"/>
-      <c r="AP110" s="25"/>
+      <c r="AN110" s="23"/>
+      <c r="AO110" s="23"/>
+      <c r="AP110" s="23"/>
       <c r="AQ110" s="10"/>
       <c r="AR110" s="10"/>
       <c r="AS110" s="10"/>
@@ -7830,9 +7826,9 @@
       <c r="AK111" s="18"/>
       <c r="AL111" s="21"/>
       <c r="AM111" s="18"/>
-      <c r="AN111" s="25"/>
-      <c r="AO111" s="25"/>
-      <c r="AP111" s="25"/>
+      <c r="AN111" s="23"/>
+      <c r="AO111" s="23"/>
+      <c r="AP111" s="23"/>
       <c r="AQ111" s="10"/>
       <c r="AR111" s="10"/>
       <c r="AS111" s="10"/>
@@ -7894,9 +7890,9 @@
       <c r="AK112" s="18"/>
       <c r="AL112" s="21"/>
       <c r="AM112" s="18"/>
-      <c r="AN112" s="25"/>
-      <c r="AO112" s="25"/>
-      <c r="AP112" s="25"/>
+      <c r="AN112" s="23"/>
+      <c r="AO112" s="23"/>
+      <c r="AP112" s="23"/>
       <c r="AQ112" s="10"/>
       <c r="AR112" s="10"/>
       <c r="AS112" s="10"/>
@@ -7958,9 +7954,9 @@
       <c r="AK113" s="18"/>
       <c r="AL113" s="21"/>
       <c r="AM113" s="18"/>
-      <c r="AN113" s="25"/>
-      <c r="AO113" s="25"/>
-      <c r="AP113" s="25"/>
+      <c r="AN113" s="23"/>
+      <c r="AO113" s="23"/>
+      <c r="AP113" s="23"/>
       <c r="AQ113" s="10"/>
       <c r="AR113" s="10"/>
       <c r="AS113" s="10"/>
@@ -8022,9 +8018,9 @@
       <c r="AK114" s="18"/>
       <c r="AL114" s="21"/>
       <c r="AM114" s="18"/>
-      <c r="AN114" s="25"/>
-      <c r="AO114" s="25"/>
-      <c r="AP114" s="25"/>
+      <c r="AN114" s="23"/>
+      <c r="AO114" s="23"/>
+      <c r="AP114" s="23"/>
       <c r="AQ114" s="10"/>
       <c r="AR114" s="10"/>
       <c r="AS114" s="10"/>
@@ -8086,9 +8082,9 @@
       <c r="AK115" s="18"/>
       <c r="AL115" s="21"/>
       <c r="AM115" s="18"/>
-      <c r="AN115" s="25"/>
-      <c r="AO115" s="25"/>
-      <c r="AP115" s="25"/>
+      <c r="AN115" s="23"/>
+      <c r="AO115" s="23"/>
+      <c r="AP115" s="23"/>
       <c r="AQ115" s="10"/>
       <c r="AR115" s="10"/>
       <c r="AS115" s="10"/>
@@ -8150,9 +8146,9 @@
       <c r="AK116" s="18"/>
       <c r="AL116" s="21"/>
       <c r="AM116" s="18"/>
-      <c r="AN116" s="25"/>
-      <c r="AO116" s="25"/>
-      <c r="AP116" s="25"/>
+      <c r="AN116" s="23"/>
+      <c r="AO116" s="23"/>
+      <c r="AP116" s="23"/>
       <c r="AQ116" s="10"/>
       <c r="AR116" s="10"/>
       <c r="AS116" s="10"/>
@@ -8214,9 +8210,9 @@
       <c r="AK117" s="18"/>
       <c r="AL117" s="21"/>
       <c r="AM117" s="18"/>
-      <c r="AN117" s="25"/>
-      <c r="AO117" s="25"/>
-      <c r="AP117" s="25"/>
+      <c r="AN117" s="23"/>
+      <c r="AO117" s="23"/>
+      <c r="AP117" s="23"/>
       <c r="AQ117" s="10"/>
       <c r="AR117" s="10"/>
       <c r="AS117" s="10"/>
@@ -8278,9 +8274,9 @@
       <c r="AK118" s="18"/>
       <c r="AL118" s="21"/>
       <c r="AM118" s="18"/>
-      <c r="AN118" s="25"/>
-      <c r="AO118" s="25"/>
-      <c r="AP118" s="25"/>
+      <c r="AN118" s="23"/>
+      <c r="AO118" s="23"/>
+      <c r="AP118" s="23"/>
       <c r="AQ118" s="10"/>
       <c r="AR118" s="10"/>
       <c r="AS118" s="10"/>
@@ -8342,9 +8338,9 @@
       <c r="AK119" s="18"/>
       <c r="AL119" s="21"/>
       <c r="AM119" s="18"/>
-      <c r="AN119" s="25"/>
-      <c r="AO119" s="25"/>
-      <c r="AP119" s="25"/>
+      <c r="AN119" s="23"/>
+      <c r="AO119" s="23"/>
+      <c r="AP119" s="23"/>
       <c r="AQ119" s="10"/>
       <c r="AR119" s="10"/>
       <c r="AS119" s="10"/>
@@ -8406,9 +8402,9 @@
       <c r="AK120" s="18"/>
       <c r="AL120" s="21"/>
       <c r="AM120" s="18"/>
-      <c r="AN120" s="25"/>
-      <c r="AO120" s="25"/>
-      <c r="AP120" s="25"/>
+      <c r="AN120" s="23"/>
+      <c r="AO120" s="23"/>
+      <c r="AP120" s="23"/>
       <c r="AQ120" s="10"/>
       <c r="AR120" s="10"/>
       <c r="AS120" s="10"/>
@@ -8470,9 +8466,9 @@
       <c r="AK121" s="18"/>
       <c r="AL121" s="21"/>
       <c r="AM121" s="18"/>
-      <c r="AN121" s="25"/>
-      <c r="AO121" s="25"/>
-      <c r="AP121" s="25"/>
+      <c r="AN121" s="23"/>
+      <c r="AO121" s="23"/>
+      <c r="AP121" s="23"/>
       <c r="AQ121" s="10"/>
       <c r="AR121" s="10"/>
       <c r="AS121" s="10"/>
@@ -8534,9 +8530,9 @@
       <c r="AK122" s="18"/>
       <c r="AL122" s="21"/>
       <c r="AM122" s="18"/>
-      <c r="AN122" s="25"/>
-      <c r="AO122" s="25"/>
-      <c r="AP122" s="25"/>
+      <c r="AN122" s="23"/>
+      <c r="AO122" s="23"/>
+      <c r="AP122" s="23"/>
       <c r="AQ122" s="10"/>
       <c r="AR122" s="10"/>
       <c r="AS122" s="10"/>
@@ -8598,9 +8594,9 @@
       <c r="AK123" s="18"/>
       <c r="AL123" s="21"/>
       <c r="AM123" s="18"/>
-      <c r="AN123" s="25"/>
-      <c r="AO123" s="25"/>
-      <c r="AP123" s="25"/>
+      <c r="AN123" s="23"/>
+      <c r="AO123" s="23"/>
+      <c r="AP123" s="23"/>
       <c r="AQ123" s="10"/>
       <c r="AR123" s="10"/>
       <c r="AS123" s="10"/>
@@ -8662,9 +8658,9 @@
       <c r="AK124" s="18"/>
       <c r="AL124" s="21"/>
       <c r="AM124" s="18"/>
-      <c r="AN124" s="25"/>
-      <c r="AO124" s="25"/>
-      <c r="AP124" s="25"/>
+      <c r="AN124" s="23"/>
+      <c r="AO124" s="23"/>
+      <c r="AP124" s="23"/>
       <c r="AQ124" s="10"/>
       <c r="AR124" s="10"/>
       <c r="AS124" s="10"/>
@@ -8726,9 +8722,9 @@
       <c r="AK125" s="18"/>
       <c r="AL125" s="21"/>
       <c r="AM125" s="18"/>
-      <c r="AN125" s="25"/>
-      <c r="AO125" s="25"/>
-      <c r="AP125" s="25"/>
+      <c r="AN125" s="23"/>
+      <c r="AO125" s="23"/>
+      <c r="AP125" s="23"/>
       <c r="AQ125" s="10"/>
       <c r="AR125" s="10"/>
       <c r="AS125" s="10"/>
@@ -8790,9 +8786,9 @@
       <c r="AK126" s="18"/>
       <c r="AL126" s="21"/>
       <c r="AM126" s="18"/>
-      <c r="AN126" s="25"/>
-      <c r="AO126" s="25"/>
-      <c r="AP126" s="25"/>
+      <c r="AN126" s="23"/>
+      <c r="AO126" s="23"/>
+      <c r="AP126" s="23"/>
       <c r="AQ126" s="10"/>
       <c r="AR126" s="10"/>
       <c r="AS126" s="10"/>
@@ -8854,9 +8850,9 @@
       <c r="AK127" s="18"/>
       <c r="AL127" s="21"/>
       <c r="AM127" s="18"/>
-      <c r="AN127" s="25"/>
-      <c r="AO127" s="25"/>
-      <c r="AP127" s="25"/>
+      <c r="AN127" s="23"/>
+      <c r="AO127" s="23"/>
+      <c r="AP127" s="23"/>
       <c r="AQ127" s="10"/>
       <c r="AR127" s="10"/>
       <c r="AS127" s="10"/>
@@ -8918,9 +8914,9 @@
       <c r="AK128" s="18"/>
       <c r="AL128" s="21"/>
       <c r="AM128" s="18"/>
-      <c r="AN128" s="25"/>
-      <c r="AO128" s="25"/>
-      <c r="AP128" s="25"/>
+      <c r="AN128" s="23"/>
+      <c r="AO128" s="23"/>
+      <c r="AP128" s="23"/>
       <c r="AQ128" s="10"/>
       <c r="AR128" s="10"/>
       <c r="AS128" s="10"/>
@@ -8982,9 +8978,9 @@
       <c r="AK129" s="18"/>
       <c r="AL129" s="21"/>
       <c r="AM129" s="18"/>
-      <c r="AN129" s="25"/>
-      <c r="AO129" s="25"/>
-      <c r="AP129" s="25"/>
+      <c r="AN129" s="23"/>
+      <c r="AO129" s="23"/>
+      <c r="AP129" s="23"/>
       <c r="AQ129" s="10"/>
       <c r="AR129" s="10"/>
       <c r="AS129" s="10"/>
@@ -9046,9 +9042,9 @@
       <c r="AK130" s="18"/>
       <c r="AL130" s="21"/>
       <c r="AM130" s="18"/>
-      <c r="AN130" s="25"/>
-      <c r="AO130" s="25"/>
-      <c r="AP130" s="25"/>
+      <c r="AN130" s="23"/>
+      <c r="AO130" s="23"/>
+      <c r="AP130" s="23"/>
       <c r="AQ130" s="10"/>
       <c r="AR130" s="10"/>
       <c r="AS130" s="10"/>
@@ -9110,9 +9106,9 @@
       <c r="AK131" s="18"/>
       <c r="AL131" s="21"/>
       <c r="AM131" s="18"/>
-      <c r="AN131" s="25"/>
-      <c r="AO131" s="25"/>
-      <c r="AP131" s="25"/>
+      <c r="AN131" s="23"/>
+      <c r="AO131" s="23"/>
+      <c r="AP131" s="23"/>
       <c r="AQ131" s="10"/>
       <c r="AR131" s="10"/>
       <c r="AS131" s="10"/>
@@ -9174,9 +9170,9 @@
       <c r="AK132" s="18"/>
       <c r="AL132" s="21"/>
       <c r="AM132" s="18"/>
-      <c r="AN132" s="25"/>
-      <c r="AO132" s="25"/>
-      <c r="AP132" s="25"/>
+      <c r="AN132" s="23"/>
+      <c r="AO132" s="23"/>
+      <c r="AP132" s="23"/>
       <c r="AQ132" s="10"/>
       <c r="AR132" s="10"/>
       <c r="AS132" s="10"/>
@@ -9238,9 +9234,9 @@
       <c r="AK133" s="18"/>
       <c r="AL133" s="21"/>
       <c r="AM133" s="18"/>
-      <c r="AN133" s="25"/>
-      <c r="AO133" s="25"/>
-      <c r="AP133" s="25"/>
+      <c r="AN133" s="23"/>
+      <c r="AO133" s="23"/>
+      <c r="AP133" s="23"/>
       <c r="AQ133" s="10"/>
       <c r="AR133" s="10"/>
       <c r="AS133" s="10"/>
@@ -9302,9 +9298,9 @@
       <c r="AK134" s="18"/>
       <c r="AL134" s="21"/>
       <c r="AM134" s="18"/>
-      <c r="AN134" s="25"/>
-      <c r="AO134" s="25"/>
-      <c r="AP134" s="25"/>
+      <c r="AN134" s="23"/>
+      <c r="AO134" s="23"/>
+      <c r="AP134" s="23"/>
       <c r="AQ134" s="10"/>
       <c r="AR134" s="10"/>
       <c r="AS134" s="10"/>
@@ -9366,9 +9362,9 @@
       <c r="AK135" s="18"/>
       <c r="AL135" s="21"/>
       <c r="AM135" s="18"/>
-      <c r="AN135" s="25"/>
-      <c r="AO135" s="25"/>
-      <c r="AP135" s="25"/>
+      <c r="AN135" s="23"/>
+      <c r="AO135" s="23"/>
+      <c r="AP135" s="23"/>
       <c r="AQ135" s="10"/>
       <c r="AR135" s="10"/>
       <c r="AS135" s="10"/>
@@ -9430,9 +9426,9 @@
       <c r="AK136" s="18"/>
       <c r="AL136" s="21"/>
       <c r="AM136" s="18"/>
-      <c r="AN136" s="25"/>
-      <c r="AO136" s="25"/>
-      <c r="AP136" s="25"/>
+      <c r="AN136" s="23"/>
+      <c r="AO136" s="23"/>
+      <c r="AP136" s="23"/>
       <c r="AQ136" s="10"/>
       <c r="AR136" s="10"/>
       <c r="AS136" s="10"/>
@@ -9494,9 +9490,9 @@
       <c r="AK137" s="18"/>
       <c r="AL137" s="21"/>
       <c r="AM137" s="18"/>
-      <c r="AN137" s="25"/>
-      <c r="AO137" s="25"/>
-      <c r="AP137" s="25"/>
+      <c r="AN137" s="23"/>
+      <c r="AO137" s="23"/>
+      <c r="AP137" s="23"/>
       <c r="AQ137" s="10"/>
       <c r="AR137" s="10"/>
       <c r="AS137" s="10"/>
@@ -9558,9 +9554,9 @@
       <c r="AK138" s="18"/>
       <c r="AL138" s="21"/>
       <c r="AM138" s="18"/>
-      <c r="AN138" s="25"/>
-      <c r="AO138" s="25"/>
-      <c r="AP138" s="25"/>
+      <c r="AN138" s="23"/>
+      <c r="AO138" s="23"/>
+      <c r="AP138" s="23"/>
       <c r="AQ138" s="10"/>
       <c r="AR138" s="10"/>
       <c r="AS138" s="10"/>
@@ -9622,9 +9618,9 @@
       <c r="AK139" s="18"/>
       <c r="AL139" s="21"/>
       <c r="AM139" s="18"/>
-      <c r="AN139" s="25"/>
-      <c r="AO139" s="25"/>
-      <c r="AP139" s="25"/>
+      <c r="AN139" s="23"/>
+      <c r="AO139" s="23"/>
+      <c r="AP139" s="23"/>
       <c r="AQ139" s="10"/>
       <c r="AR139" s="10"/>
       <c r="AS139" s="10"/>
@@ -9686,9 +9682,9 @@
       <c r="AK140" s="18"/>
       <c r="AL140" s="21"/>
       <c r="AM140" s="18"/>
-      <c r="AN140" s="25"/>
-      <c r="AO140" s="25"/>
-      <c r="AP140" s="25"/>
+      <c r="AN140" s="23"/>
+      <c r="AO140" s="23"/>
+      <c r="AP140" s="23"/>
       <c r="AQ140" s="10"/>
       <c r="AR140" s="10"/>
       <c r="AS140" s="10"/>
@@ -9750,9 +9746,9 @@
       <c r="AK141" s="18"/>
       <c r="AL141" s="21"/>
       <c r="AM141" s="18"/>
-      <c r="AN141" s="25"/>
-      <c r="AO141" s="25"/>
-      <c r="AP141" s="25"/>
+      <c r="AN141" s="23"/>
+      <c r="AO141" s="23"/>
+      <c r="AP141" s="23"/>
       <c r="AQ141" s="10"/>
       <c r="AR141" s="10"/>
       <c r="AS141" s="10"/>
@@ -9814,9 +9810,9 @@
       <c r="AK142" s="18"/>
       <c r="AL142" s="21"/>
       <c r="AM142" s="18"/>
-      <c r="AN142" s="25"/>
-      <c r="AO142" s="25"/>
-      <c r="AP142" s="25"/>
+      <c r="AN142" s="23"/>
+      <c r="AO142" s="23"/>
+      <c r="AP142" s="23"/>
       <c r="AQ142" s="10"/>
       <c r="AR142" s="10"/>
       <c r="AS142" s="10"/>
@@ -9878,9 +9874,9 @@
       <c r="AK143" s="18"/>
       <c r="AL143" s="21"/>
       <c r="AM143" s="18"/>
-      <c r="AN143" s="25"/>
-      <c r="AO143" s="25"/>
-      <c r="AP143" s="25"/>
+      <c r="AN143" s="23"/>
+      <c r="AO143" s="23"/>
+      <c r="AP143" s="23"/>
       <c r="AQ143" s="10"/>
       <c r="AR143" s="10"/>
       <c r="AS143" s="10"/>
@@ -9942,9 +9938,9 @@
       <c r="AK144" s="18"/>
       <c r="AL144" s="21"/>
       <c r="AM144" s="18"/>
-      <c r="AN144" s="25"/>
-      <c r="AO144" s="25"/>
-      <c r="AP144" s="25"/>
+      <c r="AN144" s="23"/>
+      <c r="AO144" s="23"/>
+      <c r="AP144" s="23"/>
       <c r="AQ144" s="10"/>
       <c r="AR144" s="10"/>
       <c r="AS144" s="10"/>
@@ -10006,9 +10002,9 @@
       <c r="AK145" s="18"/>
       <c r="AL145" s="21"/>
       <c r="AM145" s="18"/>
-      <c r="AN145" s="25"/>
-      <c r="AO145" s="25"/>
-      <c r="AP145" s="25"/>
+      <c r="AN145" s="23"/>
+      <c r="AO145" s="23"/>
+      <c r="AP145" s="23"/>
       <c r="AQ145" s="10"/>
       <c r="AR145" s="10"/>
       <c r="AS145" s="10"/>
@@ -10070,9 +10066,9 @@
       <c r="AK146" s="18"/>
       <c r="AL146" s="21"/>
       <c r="AM146" s="18"/>
-      <c r="AN146" s="25"/>
-      <c r="AO146" s="25"/>
-      <c r="AP146" s="25"/>
+      <c r="AN146" s="23"/>
+      <c r="AO146" s="23"/>
+      <c r="AP146" s="23"/>
       <c r="AQ146" s="10"/>
       <c r="AR146" s="10"/>
       <c r="AS146" s="10"/>
@@ -10134,9 +10130,9 @@
       <c r="AK147" s="18"/>
       <c r="AL147" s="21"/>
       <c r="AM147" s="18"/>
-      <c r="AN147" s="25"/>
-      <c r="AO147" s="25"/>
-      <c r="AP147" s="25"/>
+      <c r="AN147" s="23"/>
+      <c r="AO147" s="23"/>
+      <c r="AP147" s="23"/>
       <c r="AQ147" s="10"/>
       <c r="AR147" s="10"/>
       <c r="AS147" s="10"/>
@@ -10198,9 +10194,9 @@
       <c r="AK148" s="18"/>
       <c r="AL148" s="21"/>
       <c r="AM148" s="18"/>
-      <c r="AN148" s="25"/>
-      <c r="AO148" s="25"/>
-      <c r="AP148" s="25"/>
+      <c r="AN148" s="23"/>
+      <c r="AO148" s="23"/>
+      <c r="AP148" s="23"/>
       <c r="AQ148" s="10"/>
       <c r="AR148" s="10"/>
       <c r="AS148" s="10"/>
@@ -10262,9 +10258,9 @@
       <c r="AK149" s="18"/>
       <c r="AL149" s="21"/>
       <c r="AM149" s="18"/>
-      <c r="AN149" s="25"/>
-      <c r="AO149" s="25"/>
-      <c r="AP149" s="25"/>
+      <c r="AN149" s="23"/>
+      <c r="AO149" s="23"/>
+      <c r="AP149" s="23"/>
       <c r="AQ149" s="10"/>
       <c r="AR149" s="10"/>
       <c r="AS149" s="10"/>
@@ -10326,9 +10322,9 @@
       <c r="AK150" s="18"/>
       <c r="AL150" s="21"/>
       <c r="AM150" s="18"/>
-      <c r="AN150" s="25"/>
-      <c r="AO150" s="25"/>
-      <c r="AP150" s="25"/>
+      <c r="AN150" s="23"/>
+      <c r="AO150" s="23"/>
+      <c r="AP150" s="23"/>
       <c r="AQ150" s="10"/>
       <c r="AR150" s="10"/>
       <c r="AS150" s="10"/>
@@ -10390,9 +10386,9 @@
       <c r="AK151" s="18"/>
       <c r="AL151" s="21"/>
       <c r="AM151" s="18"/>
-      <c r="AN151" s="25"/>
-      <c r="AO151" s="25"/>
-      <c r="AP151" s="25"/>
+      <c r="AN151" s="23"/>
+      <c r="AO151" s="23"/>
+      <c r="AP151" s="23"/>
       <c r="AQ151" s="10"/>
       <c r="AR151" s="10"/>
       <c r="AS151" s="10"/>
@@ -10454,9 +10450,9 @@
       <c r="AK152" s="18"/>
       <c r="AL152" s="21"/>
       <c r="AM152" s="18"/>
-      <c r="AN152" s="25"/>
-      <c r="AO152" s="25"/>
-      <c r="AP152" s="25"/>
+      <c r="AN152" s="23"/>
+      <c r="AO152" s="23"/>
+      <c r="AP152" s="23"/>
       <c r="AQ152" s="10"/>
       <c r="AR152" s="10"/>
       <c r="AS152" s="10"/>
@@ -10518,9 +10514,9 @@
       <c r="AK153" s="18"/>
       <c r="AL153" s="21"/>
       <c r="AM153" s="18"/>
-      <c r="AN153" s="25"/>
-      <c r="AO153" s="25"/>
-      <c r="AP153" s="25"/>
+      <c r="AN153" s="23"/>
+      <c r="AO153" s="23"/>
+      <c r="AP153" s="23"/>
       <c r="AQ153" s="10"/>
       <c r="AR153" s="10"/>
       <c r="AS153" s="10"/>
@@ -10582,9 +10578,9 @@
       <c r="AK154" s="18"/>
       <c r="AL154" s="21"/>
       <c r="AM154" s="18"/>
-      <c r="AN154" s="25"/>
-      <c r="AO154" s="25"/>
-      <c r="AP154" s="25"/>
+      <c r="AN154" s="23"/>
+      <c r="AO154" s="23"/>
+      <c r="AP154" s="23"/>
       <c r="AQ154" s="10"/>
       <c r="AR154" s="10"/>
       <c r="AS154" s="10"/>
@@ -10646,9 +10642,9 @@
       <c r="AK155" s="18"/>
       <c r="AL155" s="21"/>
       <c r="AM155" s="18"/>
-      <c r="AN155" s="25"/>
-      <c r="AO155" s="25"/>
-      <c r="AP155" s="25"/>
+      <c r="AN155" s="23"/>
+      <c r="AO155" s="23"/>
+      <c r="AP155" s="23"/>
       <c r="AQ155" s="10"/>
       <c r="AR155" s="10"/>
       <c r="AS155" s="10"/>
@@ -10710,9 +10706,9 @@
       <c r="AK156" s="18"/>
       <c r="AL156" s="21"/>
       <c r="AM156" s="18"/>
-      <c r="AN156" s="25"/>
-      <c r="AO156" s="25"/>
-      <c r="AP156" s="25"/>
+      <c r="AN156" s="23"/>
+      <c r="AO156" s="23"/>
+      <c r="AP156" s="23"/>
       <c r="AQ156" s="10"/>
       <c r="AR156" s="10"/>
       <c r="AS156" s="10"/>
@@ -10774,9 +10770,9 @@
       <c r="AK157" s="18"/>
       <c r="AL157" s="21"/>
       <c r="AM157" s="18"/>
-      <c r="AN157" s="25"/>
-      <c r="AO157" s="25"/>
-      <c r="AP157" s="25"/>
+      <c r="AN157" s="23"/>
+      <c r="AO157" s="23"/>
+      <c r="AP157" s="23"/>
       <c r="AQ157" s="10"/>
       <c r="AR157" s="10"/>
       <c r="AS157" s="10"/>
@@ -10838,9 +10834,9 @@
       <c r="AK158" s="18"/>
       <c r="AL158" s="21"/>
       <c r="AM158" s="18"/>
-      <c r="AN158" s="25"/>
-      <c r="AO158" s="25"/>
-      <c r="AP158" s="25"/>
+      <c r="AN158" s="23"/>
+      <c r="AO158" s="23"/>
+      <c r="AP158" s="23"/>
       <c r="AQ158" s="10"/>
       <c r="AR158" s="10"/>
       <c r="AS158" s="10"/>
@@ -10902,9 +10898,9 @@
       <c r="AK159" s="18"/>
       <c r="AL159" s="21"/>
       <c r="AM159" s="18"/>
-      <c r="AN159" s="25"/>
-      <c r="AO159" s="25"/>
-      <c r="AP159" s="25"/>
+      <c r="AN159" s="23"/>
+      <c r="AO159" s="23"/>
+      <c r="AP159" s="23"/>
       <c r="AQ159" s="10"/>
       <c r="AR159" s="10"/>
       <c r="AS159" s="10"/>
@@ -10966,9 +10962,9 @@
       <c r="AK160" s="18"/>
       <c r="AL160" s="21"/>
       <c r="AM160" s="18"/>
-      <c r="AN160" s="25"/>
-      <c r="AO160" s="25"/>
-      <c r="AP160" s="25"/>
+      <c r="AN160" s="23"/>
+      <c r="AO160" s="23"/>
+      <c r="AP160" s="23"/>
       <c r="AQ160" s="10"/>
       <c r="AR160" s="10"/>
       <c r="AS160" s="10"/>
@@ -11030,9 +11026,9 @@
       <c r="AK161" s="18"/>
       <c r="AL161" s="21"/>
       <c r="AM161" s="18"/>
-      <c r="AN161" s="25"/>
-      <c r="AO161" s="25"/>
-      <c r="AP161" s="25"/>
+      <c r="AN161" s="23"/>
+      <c r="AO161" s="23"/>
+      <c r="AP161" s="23"/>
       <c r="AQ161" s="10"/>
       <c r="AR161" s="10"/>
       <c r="AS161" s="10"/>
@@ -11094,9 +11090,9 @@
       <c r="AK162" s="18"/>
       <c r="AL162" s="21"/>
       <c r="AM162" s="18"/>
-      <c r="AN162" s="25"/>
-      <c r="AO162" s="25"/>
-      <c r="AP162" s="25"/>
+      <c r="AN162" s="23"/>
+      <c r="AO162" s="23"/>
+      <c r="AP162" s="23"/>
       <c r="AQ162" s="10"/>
       <c r="AR162" s="10"/>
       <c r="AS162" s="10"/>
@@ -11158,9 +11154,9 @@
       <c r="AK163" s="18"/>
       <c r="AL163" s="21"/>
       <c r="AM163" s="18"/>
-      <c r="AN163" s="25"/>
-      <c r="AO163" s="25"/>
-      <c r="AP163" s="25"/>
+      <c r="AN163" s="23"/>
+      <c r="AO163" s="23"/>
+      <c r="AP163" s="23"/>
       <c r="AQ163" s="10"/>
       <c r="AR163" s="10"/>
       <c r="AS163" s="10"/>
@@ -11222,9 +11218,9 @@
       <c r="AK164" s="18"/>
       <c r="AL164" s="21"/>
       <c r="AM164" s="18"/>
-      <c r="AN164" s="25"/>
-      <c r="AO164" s="25"/>
-      <c r="AP164" s="25"/>
+      <c r="AN164" s="23"/>
+      <c r="AO164" s="23"/>
+      <c r="AP164" s="23"/>
       <c r="AQ164" s="10"/>
       <c r="AR164" s="10"/>
       <c r="AS164" s="10"/>
@@ -11286,9 +11282,9 @@
       <c r="AK165" s="18"/>
       <c r="AL165" s="21"/>
       <c r="AM165" s="18"/>
-      <c r="AN165" s="25"/>
-      <c r="AO165" s="25"/>
-      <c r="AP165" s="25"/>
+      <c r="AN165" s="23"/>
+      <c r="AO165" s="23"/>
+      <c r="AP165" s="23"/>
       <c r="AQ165" s="10"/>
       <c r="AR165" s="10"/>
       <c r="AS165" s="10"/>
@@ -11350,9 +11346,9 @@
       <c r="AK166" s="18"/>
       <c r="AL166" s="21"/>
       <c r="AM166" s="18"/>
-      <c r="AN166" s="25"/>
-      <c r="AO166" s="25"/>
-      <c r="AP166" s="25"/>
+      <c r="AN166" s="23"/>
+      <c r="AO166" s="23"/>
+      <c r="AP166" s="23"/>
       <c r="AQ166" s="10"/>
       <c r="AR166" s="10"/>
       <c r="AS166" s="10"/>
@@ -11414,9 +11410,9 @@
       <c r="AK167" s="18"/>
       <c r="AL167" s="21"/>
       <c r="AM167" s="18"/>
-      <c r="AN167" s="25"/>
-      <c r="AO167" s="25"/>
-      <c r="AP167" s="25"/>
+      <c r="AN167" s="23"/>
+      <c r="AO167" s="23"/>
+      <c r="AP167" s="23"/>
       <c r="AQ167" s="10"/>
       <c r="AR167" s="10"/>
       <c r="AS167" s="10"/>
@@ -11478,9 +11474,9 @@
       <c r="AK168" s="18"/>
       <c r="AL168" s="21"/>
       <c r="AM168" s="18"/>
-      <c r="AN168" s="25"/>
-      <c r="AO168" s="25"/>
-      <c r="AP168" s="25"/>
+      <c r="AN168" s="23"/>
+      <c r="AO168" s="23"/>
+      <c r="AP168" s="23"/>
       <c r="AQ168" s="10"/>
       <c r="AR168" s="10"/>
       <c r="AS168" s="10"/>
@@ -11542,9 +11538,9 @@
       <c r="AK169" s="18"/>
       <c r="AL169" s="21"/>
       <c r="AM169" s="18"/>
-      <c r="AN169" s="25"/>
-      <c r="AO169" s="25"/>
-      <c r="AP169" s="25"/>
+      <c r="AN169" s="23"/>
+      <c r="AO169" s="23"/>
+      <c r="AP169" s="23"/>
       <c r="AQ169" s="10"/>
       <c r="AR169" s="10"/>
       <c r="AS169" s="10"/>
@@ -11606,9 +11602,9 @@
       <c r="AK170" s="18"/>
       <c r="AL170" s="21"/>
       <c r="AM170" s="18"/>
-      <c r="AN170" s="25"/>
-      <c r="AO170" s="25"/>
-      <c r="AP170" s="25"/>
+      <c r="AN170" s="23"/>
+      <c r="AO170" s="23"/>
+      <c r="AP170" s="23"/>
       <c r="AQ170" s="10"/>
       <c r="AR170" s="10"/>
       <c r="AS170" s="10"/>
@@ -11670,9 +11666,9 @@
       <c r="AK171" s="18"/>
       <c r="AL171" s="21"/>
       <c r="AM171" s="18"/>
-      <c r="AN171" s="25"/>
-      <c r="AO171" s="25"/>
-      <c r="AP171" s="25"/>
+      <c r="AN171" s="23"/>
+      <c r="AO171" s="23"/>
+      <c r="AP171" s="23"/>
       <c r="AQ171" s="10"/>
       <c r="AR171" s="10"/>
       <c r="AS171" s="10"/>
@@ -11734,9 +11730,9 @@
       <c r="AK172" s="18"/>
       <c r="AL172" s="21"/>
       <c r="AM172" s="18"/>
-      <c r="AN172" s="25"/>
-      <c r="AO172" s="25"/>
-      <c r="AP172" s="25"/>
+      <c r="AN172" s="23"/>
+      <c r="AO172" s="23"/>
+      <c r="AP172" s="23"/>
       <c r="AQ172" s="10"/>
       <c r="AR172" s="10"/>
       <c r="AS172" s="10"/>
@@ -11798,9 +11794,9 @@
       <c r="AK173" s="18"/>
       <c r="AL173" s="21"/>
       <c r="AM173" s="18"/>
-      <c r="AN173" s="25"/>
-      <c r="AO173" s="25"/>
-      <c r="AP173" s="25"/>
+      <c r="AN173" s="23"/>
+      <c r="AO173" s="23"/>
+      <c r="AP173" s="23"/>
       <c r="AQ173" s="10"/>
       <c r="AR173" s="10"/>
       <c r="AS173" s="10"/>
@@ -11862,9 +11858,9 @@
       <c r="AK174" s="18"/>
       <c r="AL174" s="21"/>
       <c r="AM174" s="18"/>
-      <c r="AN174" s="25"/>
-      <c r="AO174" s="25"/>
-      <c r="AP174" s="25"/>
+      <c r="AN174" s="23"/>
+      <c r="AO174" s="23"/>
+      <c r="AP174" s="23"/>
       <c r="AQ174" s="10"/>
       <c r="AR174" s="10"/>
       <c r="AS174" s="10"/>
@@ -11926,9 +11922,9 @@
       <c r="AK175" s="18"/>
       <c r="AL175" s="21"/>
       <c r="AM175" s="18"/>
-      <c r="AN175" s="25"/>
-      <c r="AO175" s="25"/>
-      <c r="AP175" s="25"/>
+      <c r="AN175" s="23"/>
+      <c r="AO175" s="23"/>
+      <c r="AP175" s="23"/>
       <c r="AQ175" s="10"/>
       <c r="AR175" s="10"/>
       <c r="AS175" s="10"/>
@@ -11990,9 +11986,9 @@
       <c r="AK176" s="18"/>
       <c r="AL176" s="21"/>
       <c r="AM176" s="18"/>
-      <c r="AN176" s="25"/>
-      <c r="AO176" s="25"/>
-      <c r="AP176" s="25"/>
+      <c r="AN176" s="23"/>
+      <c r="AO176" s="23"/>
+      <c r="AP176" s="23"/>
       <c r="AQ176" s="10"/>
       <c r="AR176" s="10"/>
       <c r="AS176" s="10"/>
@@ -12054,9 +12050,9 @@
       <c r="AK177" s="18"/>
       <c r="AL177" s="21"/>
       <c r="AM177" s="18"/>
-      <c r="AN177" s="25"/>
-      <c r="AO177" s="25"/>
-      <c r="AP177" s="25"/>
+      <c r="AN177" s="23"/>
+      <c r="AO177" s="23"/>
+      <c r="AP177" s="23"/>
       <c r="AQ177" s="10"/>
       <c r="AR177" s="10"/>
       <c r="AS177" s="10"/>
@@ -12118,9 +12114,9 @@
       <c r="AK178" s="18"/>
       <c r="AL178" s="21"/>
       <c r="AM178" s="18"/>
-      <c r="AN178" s="25"/>
-      <c r="AO178" s="25"/>
-      <c r="AP178" s="25"/>
+      <c r="AN178" s="23"/>
+      <c r="AO178" s="23"/>
+      <c r="AP178" s="23"/>
       <c r="AQ178" s="10"/>
       <c r="AR178" s="10"/>
       <c r="AS178" s="10"/>
@@ -12182,9 +12178,9 @@
       <c r="AK179" s="18"/>
       <c r="AL179" s="21"/>
       <c r="AM179" s="18"/>
-      <c r="AN179" s="25"/>
-      <c r="AO179" s="25"/>
-      <c r="AP179" s="25"/>
+      <c r="AN179" s="23"/>
+      <c r="AO179" s="23"/>
+      <c r="AP179" s="23"/>
       <c r="AQ179" s="10"/>
       <c r="AR179" s="10"/>
       <c r="AS179" s="10"/>
@@ -12246,9 +12242,9 @@
       <c r="AK180" s="18"/>
       <c r="AL180" s="21"/>
       <c r="AM180" s="18"/>
-      <c r="AN180" s="25"/>
-      <c r="AO180" s="25"/>
-      <c r="AP180" s="25"/>
+      <c r="AN180" s="23"/>
+      <c r="AO180" s="23"/>
+      <c r="AP180" s="23"/>
       <c r="AQ180" s="10"/>
       <c r="AR180" s="10"/>
       <c r="AS180" s="10"/>
@@ -12310,9 +12306,9 @@
       <c r="AK181" s="18"/>
       <c r="AL181" s="21"/>
       <c r="AM181" s="18"/>
-      <c r="AN181" s="25"/>
-      <c r="AO181" s="25"/>
-      <c r="AP181" s="25"/>
+      <c r="AN181" s="23"/>
+      <c r="AO181" s="23"/>
+      <c r="AP181" s="23"/>
       <c r="AQ181" s="10"/>
       <c r="AR181" s="10"/>
       <c r="AS181" s="10"/>
@@ -12374,9 +12370,9 @@
       <c r="AK182" s="18"/>
       <c r="AL182" s="21"/>
       <c r="AM182" s="18"/>
-      <c r="AN182" s="25"/>
-      <c r="AO182" s="25"/>
-      <c r="AP182" s="25"/>
+      <c r="AN182" s="23"/>
+      <c r="AO182" s="23"/>
+      <c r="AP182" s="23"/>
       <c r="AQ182" s="10"/>
       <c r="AR182" s="10"/>
       <c r="AS182" s="10"/>
@@ -12438,9 +12434,9 @@
       <c r="AK183" s="18"/>
       <c r="AL183" s="21"/>
       <c r="AM183" s="18"/>
-      <c r="AN183" s="25"/>
-      <c r="AO183" s="25"/>
-      <c r="AP183" s="25"/>
+      <c r="AN183" s="23"/>
+      <c r="AO183" s="23"/>
+      <c r="AP183" s="23"/>
       <c r="AQ183" s="10"/>
       <c r="AR183" s="10"/>
       <c r="AS183" s="10"/>
@@ -12502,9 +12498,9 @@
       <c r="AK184" s="18"/>
       <c r="AL184" s="21"/>
       <c r="AM184" s="18"/>
-      <c r="AN184" s="25"/>
-      <c r="AO184" s="25"/>
-      <c r="AP184" s="25"/>
+      <c r="AN184" s="23"/>
+      <c r="AO184" s="23"/>
+      <c r="AP184" s="23"/>
       <c r="AQ184" s="10"/>
       <c r="AR184" s="10"/>
       <c r="AS184" s="10"/>
@@ -12566,9 +12562,9 @@
       <c r="AK185" s="18"/>
       <c r="AL185" s="21"/>
       <c r="AM185" s="18"/>
-      <c r="AN185" s="25"/>
-      <c r="AO185" s="25"/>
-      <c r="AP185" s="25"/>
+      <c r="AN185" s="23"/>
+      <c r="AO185" s="23"/>
+      <c r="AP185" s="23"/>
       <c r="AQ185" s="10"/>
       <c r="AR185" s="10"/>
       <c r="AS185" s="10"/>
@@ -12630,9 +12626,9 @@
       <c r="AK186" s="18"/>
       <c r="AL186" s="21"/>
       <c r="AM186" s="18"/>
-      <c r="AN186" s="25"/>
-      <c r="AO186" s="25"/>
-      <c r="AP186" s="25"/>
+      <c r="AN186" s="23"/>
+      <c r="AO186" s="23"/>
+      <c r="AP186" s="23"/>
       <c r="AQ186" s="10"/>
       <c r="AR186" s="10"/>
       <c r="AS186" s="10"/>
@@ -12694,9 +12690,9 @@
       <c r="AK187" s="18"/>
       <c r="AL187" s="21"/>
       <c r="AM187" s="18"/>
-      <c r="AN187" s="25"/>
-      <c r="AO187" s="25"/>
-      <c r="AP187" s="25"/>
+      <c r="AN187" s="23"/>
+      <c r="AO187" s="23"/>
+      <c r="AP187" s="23"/>
       <c r="AQ187" s="10"/>
       <c r="AR187" s="10"/>
       <c r="AS187" s="10"/>
@@ -12758,9 +12754,9 @@
       <c r="AK188" s="18"/>
       <c r="AL188" s="21"/>
       <c r="AM188" s="18"/>
-      <c r="AN188" s="25"/>
-      <c r="AO188" s="25"/>
-      <c r="AP188" s="25"/>
+      <c r="AN188" s="23"/>
+      <c r="AO188" s="23"/>
+      <c r="AP188" s="23"/>
       <c r="AQ188" s="10"/>
       <c r="AR188" s="10"/>
       <c r="AS188" s="10"/>
@@ -12822,9 +12818,9 @@
       <c r="AK189" s="18"/>
       <c r="AL189" s="21"/>
       <c r="AM189" s="18"/>
-      <c r="AN189" s="25"/>
-      <c r="AO189" s="25"/>
-      <c r="AP189" s="25"/>
+      <c r="AN189" s="23"/>
+      <c r="AO189" s="23"/>
+      <c r="AP189" s="23"/>
       <c r="AQ189" s="10"/>
       <c r="AR189" s="10"/>
       <c r="AS189" s="10"/>
@@ -12886,9 +12882,9 @@
       <c r="AK190" s="18"/>
       <c r="AL190" s="21"/>
       <c r="AM190" s="18"/>
-      <c r="AN190" s="25"/>
-      <c r="AO190" s="25"/>
-      <c r="AP190" s="25"/>
+      <c r="AN190" s="23"/>
+      <c r="AO190" s="23"/>
+      <c r="AP190" s="23"/>
       <c r="AQ190" s="10"/>
       <c r="AR190" s="10"/>
       <c r="AS190" s="10"/>
@@ -12950,9 +12946,9 @@
       <c r="AK191" s="18"/>
       <c r="AL191" s="21"/>
       <c r="AM191" s="18"/>
-      <c r="AN191" s="25"/>
-      <c r="AO191" s="25"/>
-      <c r="AP191" s="25"/>
+      <c r="AN191" s="23"/>
+      <c r="AO191" s="23"/>
+      <c r="AP191" s="23"/>
       <c r="AQ191" s="10"/>
       <c r="AR191" s="10"/>
       <c r="AS191" s="10"/>
@@ -13014,9 +13010,9 @@
       <c r="AK192" s="18"/>
       <c r="AL192" s="21"/>
       <c r="AM192" s="18"/>
-      <c r="AN192" s="25"/>
-      <c r="AO192" s="25"/>
-      <c r="AP192" s="25"/>
+      <c r="AN192" s="23"/>
+      <c r="AO192" s="23"/>
+      <c r="AP192" s="23"/>
       <c r="AQ192" s="10"/>
       <c r="AR192" s="10"/>
       <c r="AS192" s="10"/>
@@ -13078,9 +13074,9 @@
       <c r="AK193" s="18"/>
       <c r="AL193" s="21"/>
       <c r="AM193" s="18"/>
-      <c r="AN193" s="25"/>
-      <c r="AO193" s="25"/>
-      <c r="AP193" s="25"/>
+      <c r="AN193" s="23"/>
+      <c r="AO193" s="23"/>
+      <c r="AP193" s="23"/>
       <c r="AQ193" s="10"/>
       <c r="AR193" s="10"/>
       <c r="AS193" s="10"/>
@@ -13142,9 +13138,9 @@
       <c r="AK194" s="18"/>
       <c r="AL194" s="21"/>
       <c r="AM194" s="18"/>
-      <c r="AN194" s="25"/>
-      <c r="AO194" s="25"/>
-      <c r="AP194" s="25"/>
+      <c r="AN194" s="23"/>
+      <c r="AO194" s="23"/>
+      <c r="AP194" s="23"/>
       <c r="AQ194" s="10"/>
       <c r="AR194" s="10"/>
       <c r="AS194" s="10"/>
@@ -13206,9 +13202,9 @@
       <c r="AK195" s="18"/>
       <c r="AL195" s="21"/>
       <c r="AM195" s="18"/>
-      <c r="AN195" s="25"/>
-      <c r="AO195" s="25"/>
-      <c r="AP195" s="25"/>
+      <c r="AN195" s="23"/>
+      <c r="AO195" s="23"/>
+      <c r="AP195" s="23"/>
       <c r="AQ195" s="10"/>
       <c r="AR195" s="10"/>
       <c r="AS195" s="10"/>
@@ -13270,9 +13266,9 @@
       <c r="AK196" s="18"/>
       <c r="AL196" s="21"/>
       <c r="AM196" s="18"/>
-      <c r="AN196" s="25"/>
-      <c r="AO196" s="25"/>
-      <c r="AP196" s="25"/>
+      <c r="AN196" s="23"/>
+      <c r="AO196" s="23"/>
+      <c r="AP196" s="23"/>
       <c r="AQ196" s="10"/>
       <c r="AR196" s="10"/>
       <c r="AS196" s="10"/>
@@ -13334,9 +13330,9 @@
       <c r="AK197" s="18"/>
       <c r="AL197" s="21"/>
       <c r="AM197" s="18"/>
-      <c r="AN197" s="25"/>
-      <c r="AO197" s="25"/>
-      <c r="AP197" s="25"/>
+      <c r="AN197" s="23"/>
+      <c r="AO197" s="23"/>
+      <c r="AP197" s="23"/>
       <c r="AQ197" s="10"/>
       <c r="AR197" s="10"/>
       <c r="AS197" s="10"/>
@@ -13398,9 +13394,9 @@
       <c r="AK198" s="18"/>
       <c r="AL198" s="21"/>
       <c r="AM198" s="18"/>
-      <c r="AN198" s="25"/>
-      <c r="AO198" s="25"/>
-      <c r="AP198" s="25"/>
+      <c r="AN198" s="23"/>
+      <c r="AO198" s="23"/>
+      <c r="AP198" s="23"/>
       <c r="AQ198" s="10"/>
       <c r="AR198" s="10"/>
       <c r="AS198" s="10"/>
@@ -13462,9 +13458,9 @@
       <c r="AK199" s="18"/>
       <c r="AL199" s="21"/>
       <c r="AM199" s="18"/>
-      <c r="AN199" s="25"/>
-      <c r="AO199" s="25"/>
-      <c r="AP199" s="25"/>
+      <c r="AN199" s="23"/>
+      <c r="AO199" s="23"/>
+      <c r="AP199" s="23"/>
       <c r="AQ199" s="10"/>
       <c r="AR199" s="10"/>
       <c r="AS199" s="10"/>
@@ -13526,9 +13522,9 @@
       <c r="AK200" s="18"/>
       <c r="AL200" s="21"/>
       <c r="AM200" s="18"/>
-      <c r="AN200" s="25"/>
-      <c r="AO200" s="25"/>
-      <c r="AP200" s="25"/>
+      <c r="AN200" s="23"/>
+      <c r="AO200" s="23"/>
+      <c r="AP200" s="23"/>
       <c r="AQ200" s="10"/>
       <c r="AR200" s="10"/>
       <c r="AS200" s="10"/>
@@ -13590,9 +13586,9 @@
       <c r="AK201" s="18"/>
       <c r="AL201" s="21"/>
       <c r="AM201" s="18"/>
-      <c r="AN201" s="25"/>
-      <c r="AO201" s="25"/>
-      <c r="AP201" s="25"/>
+      <c r="AN201" s="23"/>
+      <c r="AO201" s="23"/>
+      <c r="AP201" s="23"/>
       <c r="AQ201" s="10"/>
       <c r="AR201" s="10"/>
       <c r="AS201" s="10"/>
@@ -13654,9 +13650,9 @@
       <c r="AK202" s="18"/>
       <c r="AL202" s="21"/>
       <c r="AM202" s="18"/>
-      <c r="AN202" s="25"/>
-      <c r="AO202" s="25"/>
-      <c r="AP202" s="25"/>
+      <c r="AN202" s="23"/>
+      <c r="AO202" s="23"/>
+      <c r="AP202" s="23"/>
       <c r="AQ202" s="10"/>
       <c r="AR202" s="10"/>
       <c r="AS202" s="10"/>
@@ -13718,9 +13714,9 @@
       <c r="AK203" s="18"/>
       <c r="AL203" s="21"/>
       <c r="AM203" s="18"/>
-      <c r="AN203" s="25"/>
-      <c r="AO203" s="25"/>
-      <c r="AP203" s="25"/>
+      <c r="AN203" s="23"/>
+      <c r="AO203" s="23"/>
+      <c r="AP203" s="23"/>
       <c r="AQ203" s="10"/>
       <c r="AR203" s="10"/>
       <c r="AS203" s="10"/>
@@ -13782,9 +13778,9 @@
       <c r="AK204" s="18"/>
       <c r="AL204" s="21"/>
       <c r="AM204" s="18"/>
-      <c r="AN204" s="25"/>
-      <c r="AO204" s="25"/>
-      <c r="AP204" s="25"/>
+      <c r="AN204" s="23"/>
+      <c r="AO204" s="23"/>
+      <c r="AP204" s="23"/>
       <c r="AQ204" s="10"/>
       <c r="AR204" s="10"/>
       <c r="AS204" s="10"/>
@@ -13846,9 +13842,9 @@
       <c r="AK205" s="18"/>
       <c r="AL205" s="21"/>
       <c r="AM205" s="18"/>
-      <c r="AN205" s="25"/>
-      <c r="AO205" s="25"/>
-      <c r="AP205" s="25"/>
+      <c r="AN205" s="23"/>
+      <c r="AO205" s="23"/>
+      <c r="AP205" s="23"/>
       <c r="AQ205" s="10"/>
       <c r="AR205" s="10"/>
       <c r="AS205" s="10"/>
@@ -13910,9 +13906,9 @@
       <c r="AK206" s="18"/>
       <c r="AL206" s="21"/>
       <c r="AM206" s="18"/>
-      <c r="AN206" s="25"/>
-      <c r="AO206" s="25"/>
-      <c r="AP206" s="25"/>
+      <c r="AN206" s="23"/>
+      <c r="AO206" s="23"/>
+      <c r="AP206" s="23"/>
       <c r="AQ206" s="10"/>
       <c r="AR206" s="10"/>
       <c r="AS206" s="10"/>
@@ -13974,9 +13970,9 @@
       <c r="AK207" s="18"/>
       <c r="AL207" s="21"/>
       <c r="AM207" s="18"/>
-      <c r="AN207" s="25"/>
-      <c r="AO207" s="25"/>
-      <c r="AP207" s="25"/>
+      <c r="AN207" s="23"/>
+      <c r="AO207" s="23"/>
+      <c r="AP207" s="23"/>
       <c r="AQ207" s="10"/>
       <c r="AR207" s="10"/>
       <c r="AS207" s="10"/>
@@ -14038,9 +14034,9 @@
       <c r="AK208" s="18"/>
       <c r="AL208" s="21"/>
       <c r="AM208" s="18"/>
-      <c r="AN208" s="25"/>
-      <c r="AO208" s="25"/>
-      <c r="AP208" s="25"/>
+      <c r="AN208" s="23"/>
+      <c r="AO208" s="23"/>
+      <c r="AP208" s="23"/>
       <c r="AQ208" s="10"/>
       <c r="AR208" s="10"/>
       <c r="AS208" s="10"/>
@@ -14102,9 +14098,9 @@
       <c r="AK209" s="18"/>
       <c r="AL209" s="21"/>
       <c r="AM209" s="18"/>
-      <c r="AN209" s="25"/>
-      <c r="AO209" s="25"/>
-      <c r="AP209" s="25"/>
+      <c r="AN209" s="23"/>
+      <c r="AO209" s="23"/>
+      <c r="AP209" s="23"/>
       <c r="AQ209" s="10"/>
       <c r="AR209" s="10"/>
       <c r="AS209" s="10"/>
@@ -14166,9 +14162,9 @@
       <c r="AK210" s="18"/>
       <c r="AL210" s="21"/>
       <c r="AM210" s="18"/>
-      <c r="AN210" s="25"/>
-      <c r="AO210" s="25"/>
-      <c r="AP210" s="25"/>
+      <c r="AN210" s="23"/>
+      <c r="AO210" s="23"/>
+      <c r="AP210" s="23"/>
       <c r="AQ210" s="10"/>
       <c r="AR210" s="10"/>
       <c r="AS210" s="10"/>
@@ -14230,9 +14226,9 @@
       <c r="AK211" s="18"/>
       <c r="AL211" s="21"/>
       <c r="AM211" s="18"/>
-      <c r="AN211" s="25"/>
-      <c r="AO211" s="25"/>
-      <c r="AP211" s="25"/>
+      <c r="AN211" s="23"/>
+      <c r="AO211" s="23"/>
+      <c r="AP211" s="23"/>
       <c r="AQ211" s="10"/>
       <c r="AR211" s="10"/>
       <c r="AS211" s="10"/>
@@ -14294,9 +14290,9 @@
       <c r="AK212" s="18"/>
       <c r="AL212" s="21"/>
       <c r="AM212" s="18"/>
-      <c r="AN212" s="25"/>
-      <c r="AO212" s="25"/>
-      <c r="AP212" s="25"/>
+      <c r="AN212" s="23"/>
+      <c r="AO212" s="23"/>
+      <c r="AP212" s="23"/>
       <c r="AQ212" s="10"/>
       <c r="AR212" s="10"/>
       <c r="AS212" s="10"/>
@@ -14358,9 +14354,9 @@
       <c r="AK213" s="18"/>
       <c r="AL213" s="21"/>
       <c r="AM213" s="18"/>
-      <c r="AN213" s="25"/>
-      <c r="AO213" s="25"/>
-      <c r="AP213" s="25"/>
+      <c r="AN213" s="23"/>
+      <c r="AO213" s="23"/>
+      <c r="AP213" s="23"/>
       <c r="AQ213" s="10"/>
       <c r="AR213" s="10"/>
       <c r="AS213" s="10"/>
@@ -14422,9 +14418,9 @@
       <c r="AK214" s="18"/>
       <c r="AL214" s="21"/>
       <c r="AM214" s="18"/>
-      <c r="AN214" s="25"/>
-      <c r="AO214" s="25"/>
-      <c r="AP214" s="25"/>
+      <c r="AN214" s="23"/>
+      <c r="AO214" s="23"/>
+      <c r="AP214" s="23"/>
       <c r="AQ214" s="10"/>
       <c r="AR214" s="10"/>
       <c r="AS214" s="10"/>
@@ -14486,9 +14482,9 @@
       <c r="AK215" s="18"/>
       <c r="AL215" s="21"/>
       <c r="AM215" s="18"/>
-      <c r="AN215" s="25"/>
-      <c r="AO215" s="25"/>
-      <c r="AP215" s="25"/>
+      <c r="AN215" s="23"/>
+      <c r="AO215" s="23"/>
+      <c r="AP215" s="23"/>
       <c r="AQ215" s="10"/>
       <c r="AR215" s="10"/>
       <c r="AS215" s="10"/>
@@ -14550,9 +14546,9 @@
       <c r="AK216" s="18"/>
       <c r="AL216" s="21"/>
       <c r="AM216" s="18"/>
-      <c r="AN216" s="25"/>
-      <c r="AO216" s="25"/>
-      <c r="AP216" s="25"/>
+      <c r="AN216" s="23"/>
+      <c r="AO216" s="23"/>
+      <c r="AP216" s="23"/>
       <c r="AQ216" s="10"/>
       <c r="AR216" s="10"/>
       <c r="AS216" s="10"/>
@@ -14614,9 +14610,9 @@
       <c r="AK217" s="18"/>
       <c r="AL217" s="21"/>
       <c r="AM217" s="18"/>
-      <c r="AN217" s="25"/>
-      <c r="AO217" s="25"/>
-      <c r="AP217" s="25"/>
+      <c r="AN217" s="23"/>
+      <c r="AO217" s="23"/>
+      <c r="AP217" s="23"/>
       <c r="AQ217" s="10"/>
       <c r="AR217" s="10"/>
       <c r="AS217" s="10"/>
@@ -14678,9 +14674,9 @@
       <c r="AK218" s="18"/>
       <c r="AL218" s="21"/>
       <c r="AM218" s="18"/>
-      <c r="AN218" s="25"/>
-      <c r="AO218" s="25"/>
-      <c r="AP218" s="25"/>
+      <c r="AN218" s="23"/>
+      <c r="AO218" s="23"/>
+      <c r="AP218" s="23"/>
       <c r="AQ218" s="10"/>
       <c r="AR218" s="10"/>
       <c r="AS218" s="10"/>
@@ -14742,9 +14738,9 @@
       <c r="AK219" s="18"/>
       <c r="AL219" s="21"/>
       <c r="AM219" s="18"/>
-      <c r="AN219" s="25"/>
-      <c r="AO219" s="25"/>
-      <c r="AP219" s="25"/>
+      <c r="AN219" s="23"/>
+      <c r="AO219" s="23"/>
+      <c r="AP219" s="23"/>
       <c r="AQ219" s="10"/>
       <c r="AR219" s="10"/>
       <c r="AS219" s="10"/>
@@ -14806,9 +14802,9 @@
       <c r="AK220" s="18"/>
       <c r="AL220" s="21"/>
       <c r="AM220" s="18"/>
-      <c r="AN220" s="25"/>
-      <c r="AO220" s="25"/>
-      <c r="AP220" s="25"/>
+      <c r="AN220" s="23"/>
+      <c r="AO220" s="23"/>
+      <c r="AP220" s="23"/>
       <c r="AQ220" s="10"/>
       <c r="AR220" s="10"/>
       <c r="AS220" s="10"/>

</xml_diff>